<commit_message>
[MS-OUTSPS]: Add new cases for major changes in RepeatPattern
</commit_message>
<xml_diff>
--- a/SharePoint/Docs/MS-OUTSPS/MS-OUTSPS_RequirementSpecification.xlsx
+++ b/SharePoint/Docs/MS-OUTSPS/MS-OUTSPS_RequirementSpecification.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8146" uniqueCount="2509">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8118" uniqueCount="2495">
   <si>
     <t>Req ID</t>
   </si>
@@ -7794,27 +7794,6 @@
     <t>[In Appendix B: Product Behavior] Implementation does interpret it as true if the attribute weekly.sa is present. (Windows® SharePoint® Services 3.0 and above products follow this behavior.)</t>
   </si>
   <si>
-    <t>Verified by derived requirement: MS-OUTSPS_R90381.</t>
-  </si>
-  <si>
-    <t>Verified by derived requirement: MS-OUTSPS_R90391.</t>
-  </si>
-  <si>
-    <t>Verified by derived requirement: MS-OUTSPS_R90401.</t>
-  </si>
-  <si>
-    <t>Verified by derived requirement: MS-OUTSPS_R90411.</t>
-  </si>
-  <si>
-    <t>Verified by derived requirement: MS-OUTSPS_R90421.</t>
-  </si>
-  <si>
-    <t>Verified by derived requirement: MS-OUTSPS_R90431.</t>
-  </si>
-  <si>
-    <t>Verified by derived requirement: MS-OUTSPS_R90441.</t>
-  </si>
-  <si>
     <t>MS-OUTSPS_R9050</t>
   </si>
   <si>
@@ -7918,27 +7897,6 @@
   </si>
   <si>
     <t>[In Appendix B: Product Behavior] Implementation does interpret it as true if the attribute monthlyByDay.sa is present. (Windows® SharePoint® Services 3.0 and above products follow this behavior.)</t>
-  </si>
-  <si>
-    <t>Verified by derived requirement: MS-OUTSPS_R90501.</t>
-  </si>
-  <si>
-    <t>Verified by derived requirement: MS-OUTSPS_R90511.</t>
-  </si>
-  <si>
-    <t>Verified by derived requirement: MS-OUTSPS_R90521.</t>
-  </si>
-  <si>
-    <t>Verified by derived requirement: MS-OUTSPS_R90531.</t>
-  </si>
-  <si>
-    <t>Verified by derived requirement: MS-OUTSPS_R90541.</t>
-  </si>
-  <si>
-    <t>Verified by derived requirement: MS-OUTSPS_R90551.</t>
-  </si>
-  <si>
-    <t>Verified by derived requirement: MS-OUTSPS_R90561.</t>
   </si>
   <si>
     <t>[In TimeZoneXML complex type]The TimeZoneXML complex type contains a TimeZoneRule (section 2.2.4.6) to define a time zone.
@@ -11715,7 +11673,7 @@
         <v>15</v>
       </c>
       <c r="H65" s="46" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="I65" s="48"/>
       <c r="J65" s="27"/>
@@ -11771,9 +11729,7 @@
       <c r="H67" s="46" t="s">
         <v>17</v>
       </c>
-      <c r="I67" s="42" t="s">
-        <v>2410</v>
-      </c>
+      <c r="I67" s="42"/>
       <c r="J67" s="27"/>
       <c r="K67" s="27"/>
     </row>
@@ -11827,9 +11783,7 @@
       <c r="H69" s="46" t="s">
         <v>17</v>
       </c>
-      <c r="I69" s="42" t="s">
-        <v>2411</v>
-      </c>
+      <c r="I69" s="42"/>
       <c r="J69" s="27"/>
       <c r="K69" s="27"/>
     </row>
@@ -11883,9 +11837,7 @@
       <c r="H71" s="46" t="s">
         <v>17</v>
       </c>
-      <c r="I71" s="42" t="s">
-        <v>2412</v>
-      </c>
+      <c r="I71" s="42"/>
       <c r="J71" s="27"/>
       <c r="K71" s="27"/>
     </row>
@@ -11939,9 +11891,7 @@
       <c r="H73" s="46" t="s">
         <v>17</v>
       </c>
-      <c r="I73" s="42" t="s">
-        <v>2413</v>
-      </c>
+      <c r="I73" s="42"/>
       <c r="J73" s="27"/>
       <c r="K73" s="27"/>
     </row>
@@ -11995,9 +11945,7 @@
       <c r="H75" s="46" t="s">
         <v>17</v>
       </c>
-      <c r="I75" s="42" t="s">
-        <v>2414</v>
-      </c>
+      <c r="I75" s="42"/>
       <c r="J75" s="27"/>
       <c r="K75" s="27"/>
     </row>
@@ -12051,9 +11999,7 @@
       <c r="H77" s="46" t="s">
         <v>17</v>
       </c>
-      <c r="I77" s="42" t="s">
-        <v>2415</v>
-      </c>
+      <c r="I77" s="42"/>
       <c r="J77" s="27"/>
       <c r="K77" s="27"/>
     </row>
@@ -12107,9 +12053,7 @@
       <c r="H79" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="I79" s="42" t="s">
-        <v>2416</v>
-      </c>
+      <c r="I79" s="42"/>
       <c r="J79" s="27"/>
       <c r="K79" s="27"/>
     </row>
@@ -12304,13 +12248,13 @@
     </row>
     <row r="87" spans="1:11" s="24" customFormat="1" ht="30">
       <c r="A87" s="51" t="s">
-        <v>2417</v>
+        <v>2410</v>
       </c>
       <c r="B87" s="47" t="s">
         <v>91</v>
       </c>
       <c r="C87" s="31" t="s">
-        <v>2424</v>
+        <v>2417</v>
       </c>
       <c r="D87" s="46"/>
       <c r="E87" s="27" t="s">
@@ -12325,9 +12269,7 @@
       <c r="H87" s="46" t="s">
         <v>17</v>
       </c>
-      <c r="I87" s="42" t="s">
-        <v>2452</v>
-      </c>
+      <c r="I87" s="42"/>
       <c r="J87" s="27"/>
       <c r="K87" s="27"/>
     </row>
@@ -12360,13 +12302,13 @@
     </row>
     <row r="89" spans="1:11" s="24" customFormat="1" ht="30">
       <c r="A89" s="51" t="s">
-        <v>2418</v>
+        <v>2411</v>
       </c>
       <c r="B89" s="47" t="s">
         <v>91</v>
       </c>
       <c r="C89" s="31" t="s">
-        <v>2425</v>
+        <v>2418</v>
       </c>
       <c r="D89" s="46"/>
       <c r="E89" s="27" t="s">
@@ -12381,9 +12323,7 @@
       <c r="H89" s="46" t="s">
         <v>17</v>
       </c>
-      <c r="I89" s="42" t="s">
-        <v>2453</v>
-      </c>
+      <c r="I89" s="42"/>
       <c r="J89" s="27"/>
       <c r="K89" s="27"/>
     </row>
@@ -12416,13 +12356,13 @@
     </row>
     <row r="91" spans="1:11" s="24" customFormat="1" ht="30">
       <c r="A91" s="51" t="s">
-        <v>2419</v>
+        <v>2412</v>
       </c>
       <c r="B91" s="47" t="s">
         <v>91</v>
       </c>
       <c r="C91" s="31" t="s">
-        <v>2426</v>
+        <v>2419</v>
       </c>
       <c r="D91" s="46"/>
       <c r="E91" s="27" t="s">
@@ -12437,9 +12377,7 @@
       <c r="H91" s="46" t="s">
         <v>17</v>
       </c>
-      <c r="I91" s="42" t="s">
-        <v>2454</v>
-      </c>
+      <c r="I91" s="42"/>
       <c r="J91" s="27"/>
       <c r="K91" s="27"/>
     </row>
@@ -12472,13 +12410,13 @@
     </row>
     <row r="93" spans="1:11" s="24" customFormat="1" ht="30">
       <c r="A93" s="51" t="s">
-        <v>2420</v>
+        <v>2413</v>
       </c>
       <c r="B93" s="47" t="s">
         <v>91</v>
       </c>
       <c r="C93" s="31" t="s">
-        <v>2427</v>
+        <v>2420</v>
       </c>
       <c r="D93" s="46"/>
       <c r="E93" s="27" t="s">
@@ -12493,9 +12431,7 @@
       <c r="H93" s="46" t="s">
         <v>17</v>
       </c>
-      <c r="I93" s="42" t="s">
-        <v>2455</v>
-      </c>
+      <c r="I93" s="42"/>
       <c r="J93" s="27"/>
       <c r="K93" s="27"/>
     </row>
@@ -12528,13 +12464,13 @@
     </row>
     <row r="95" spans="1:11" s="24" customFormat="1" ht="30">
       <c r="A95" s="51" t="s">
-        <v>2421</v>
+        <v>2414</v>
       </c>
       <c r="B95" s="47" t="s">
         <v>91</v>
       </c>
       <c r="C95" s="31" t="s">
-        <v>2428</v>
+        <v>2421</v>
       </c>
       <c r="D95" s="46"/>
       <c r="E95" s="27" t="s">
@@ -12549,9 +12485,7 @@
       <c r="H95" s="46" t="s">
         <v>17</v>
       </c>
-      <c r="I95" s="42" t="s">
-        <v>2456</v>
-      </c>
+      <c r="I95" s="42"/>
       <c r="J95" s="27"/>
       <c r="K95" s="27"/>
     </row>
@@ -12584,13 +12518,13 @@
     </row>
     <row r="97" spans="1:11" s="24" customFormat="1" ht="30">
       <c r="A97" s="51" t="s">
-        <v>2422</v>
+        <v>2415</v>
       </c>
       <c r="B97" s="47" t="s">
         <v>91</v>
       </c>
       <c r="C97" s="31" t="s">
-        <v>2429</v>
+        <v>2422</v>
       </c>
       <c r="D97" s="46"/>
       <c r="E97" s="27" t="s">
@@ -12605,9 +12539,7 @@
       <c r="H97" s="46" t="s">
         <v>17</v>
       </c>
-      <c r="I97" s="42" t="s">
-        <v>2457</v>
-      </c>
+      <c r="I97" s="42"/>
       <c r="J97" s="27"/>
       <c r="K97" s="27"/>
     </row>
@@ -12640,13 +12572,13 @@
     </row>
     <row r="99" spans="1:11" s="24" customFormat="1" ht="30">
       <c r="A99" s="51" t="s">
-        <v>2423</v>
+        <v>2416</v>
       </c>
       <c r="B99" s="47" t="s">
         <v>91</v>
       </c>
       <c r="C99" s="31" t="s">
-        <v>2430</v>
+        <v>2423</v>
       </c>
       <c r="D99" s="46"/>
       <c r="E99" s="27" t="s">
@@ -12661,9 +12593,7 @@
       <c r="H99" s="46" t="s">
         <v>17</v>
       </c>
-      <c r="I99" s="42" t="s">
-        <v>2458</v>
-      </c>
+      <c r="I99" s="42"/>
       <c r="J99" s="27"/>
       <c r="K99" s="27"/>
     </row>
@@ -13512,7 +13442,7 @@
         <v>180</v>
       </c>
       <c r="C131" s="31" t="s">
-        <v>2459</v>
+        <v>2445</v>
       </c>
       <c r="D131" s="27"/>
       <c r="E131" s="27" t="s">
@@ -13566,7 +13496,7 @@
         <v>183</v>
       </c>
       <c r="C133" s="31" t="s">
-        <v>2460</v>
+        <v>2446</v>
       </c>
       <c r="D133" s="27"/>
       <c r="E133" s="27" t="s">
@@ -13892,13 +13822,13 @@
     </row>
     <row r="145" spans="1:11" s="24" customFormat="1" ht="30">
       <c r="A145" s="46" t="s">
-        <v>2461</v>
+        <v>2447</v>
       </c>
       <c r="B145" s="47" t="s">
         <v>183</v>
       </c>
       <c r="C145" s="31" t="s">
-        <v>2462</v>
+        <v>2448</v>
       </c>
       <c r="D145" s="46"/>
       <c r="E145" s="46" t="s">
@@ -13914,7 +13844,7 @@
         <v>17</v>
       </c>
       <c r="I145" s="42" t="s">
-        <v>2466</v>
+        <v>2452</v>
       </c>
       <c r="J145" s="27"/>
       <c r="K145" s="27"/>
@@ -16600,7 +16530,7 @@
         <v>319</v>
       </c>
       <c r="C245" s="31" t="s">
-        <v>2467</v>
+        <v>2453</v>
       </c>
       <c r="D245" s="27"/>
       <c r="E245" s="27" t="s">
@@ -19223,7 +19153,7 @@
         <v>416</v>
       </c>
       <c r="C342" s="31" t="s">
-        <v>2468</v>
+        <v>2454</v>
       </c>
       <c r="D342" s="27"/>
       <c r="E342" s="27" t="s">
@@ -21329,7 +21259,7 @@
         <v>510</v>
       </c>
       <c r="C420" s="31" t="s">
-        <v>2469</v>
+        <v>2455</v>
       </c>
       <c r="D420" s="27"/>
       <c r="E420" s="27" t="s">
@@ -21545,7 +21475,7 @@
         <v>526</v>
       </c>
       <c r="C428" s="42" t="s">
-        <v>2467</v>
+        <v>2453</v>
       </c>
       <c r="D428" s="35"/>
       <c r="E428" s="27" t="s">
@@ -22820,7 +22750,7 @@
         <v>578</v>
       </c>
       <c r="C475" s="31" t="s">
-        <v>2508</v>
+        <v>2494</v>
       </c>
       <c r="D475" s="27"/>
       <c r="E475" s="27" t="s">
@@ -23144,7 +23074,7 @@
         <v>591</v>
       </c>
       <c r="C487" s="31" t="s">
-        <v>2470</v>
+        <v>2456</v>
       </c>
       <c r="D487" s="27"/>
       <c r="E487" s="27" t="s">
@@ -23360,7 +23290,7 @@
         <v>599</v>
       </c>
       <c r="C495" s="31" t="s">
-        <v>2471</v>
+        <v>2457</v>
       </c>
       <c r="D495" s="27"/>
       <c r="E495" s="27" t="s">
@@ -24386,7 +24316,7 @@
         <v>620</v>
       </c>
       <c r="C533" s="31" t="s">
-        <v>2472</v>
+        <v>2458</v>
       </c>
       <c r="D533" s="27"/>
       <c r="E533" s="27" t="s">
@@ -24785,13 +24715,13 @@
     </row>
     <row r="548" spans="1:11" s="24" customFormat="1">
       <c r="A548" s="51" t="s">
-        <v>2473</v>
+        <v>2459</v>
       </c>
       <c r="B548" s="43" t="s">
         <v>644</v>
       </c>
       <c r="C548" s="31" t="s">
-        <v>2474</v>
+        <v>2460</v>
       </c>
       <c r="D548" s="46"/>
       <c r="E548" s="27" t="s">
@@ -25034,7 +24964,7 @@
         <v>644</v>
       </c>
       <c r="C557" s="31" t="s">
-        <v>2475</v>
+        <v>2461</v>
       </c>
       <c r="D557" s="27"/>
       <c r="E557" s="27" t="s">
@@ -25815,13 +25745,13 @@
     </row>
     <row r="586" spans="1:11" s="24" customFormat="1">
       <c r="A586" s="51" t="s">
-        <v>2476</v>
+        <v>2462</v>
       </c>
       <c r="B586" s="47" t="s">
         <v>644</v>
       </c>
       <c r="C586" s="31" t="s">
-        <v>2477</v>
+        <v>2463</v>
       </c>
       <c r="D586" s="46"/>
       <c r="E586" s="27" t="s">
@@ -26982,7 +26912,7 @@
         <v>706</v>
       </c>
       <c r="C629" s="31" t="s">
-        <v>2478</v>
+        <v>2464</v>
       </c>
       <c r="D629" s="27"/>
       <c r="E629" s="27" t="s">
@@ -27003,13 +26933,13 @@
     </row>
     <row r="630" spans="1:11" s="24" customFormat="1" ht="30">
       <c r="A630" s="51" t="s">
-        <v>2479</v>
+        <v>2465</v>
       </c>
       <c r="B630" s="47" t="s">
         <v>706</v>
       </c>
       <c r="C630" s="31" t="s">
-        <v>2480</v>
+        <v>2466</v>
       </c>
       <c r="D630" s="46"/>
       <c r="E630" s="27" t="s">
@@ -27036,7 +26966,7 @@
         <v>706</v>
       </c>
       <c r="C631" s="31" t="s">
-        <v>2481</v>
+        <v>2467</v>
       </c>
       <c r="D631" s="27"/>
       <c r="E631" s="27" t="s">
@@ -27495,7 +27425,7 @@
         <v>706</v>
       </c>
       <c r="C648" s="31" t="s">
-        <v>2482</v>
+        <v>2468</v>
       </c>
       <c r="D648" s="27"/>
       <c r="E648" s="27" t="s">
@@ -27511,7 +27441,7 @@
         <v>17</v>
       </c>
       <c r="I648" s="29" t="s">
-        <v>2488</v>
+        <v>2474</v>
       </c>
       <c r="J648" s="27"/>
       <c r="K648" s="27"/>
@@ -27632,7 +27562,7 @@
         <v>706</v>
       </c>
       <c r="C653" s="31" t="s">
-        <v>2489</v>
+        <v>2475</v>
       </c>
       <c r="D653" s="27"/>
       <c r="E653" s="27" t="s">
@@ -32477,7 +32407,7 @@
         <v>802</v>
       </c>
       <c r="C832" s="31" t="s">
-        <v>2490</v>
+        <v>2476</v>
       </c>
       <c r="D832" s="27"/>
       <c r="E832" s="27" t="s">
@@ -33584,7 +33514,7 @@
         <v>802</v>
       </c>
       <c r="C873" s="31" t="s">
-        <v>2491</v>
+        <v>2477</v>
       </c>
       <c r="D873" s="27"/>
       <c r="E873" s="27" t="s">
@@ -33665,7 +33595,7 @@
         <v>802</v>
       </c>
       <c r="C876" s="31" t="s">
-        <v>2492</v>
+        <v>2478</v>
       </c>
       <c r="D876" s="27"/>
       <c r="E876" s="27" t="s">
@@ -35717,7 +35647,7 @@
         <v>1054</v>
       </c>
       <c r="C952" s="42" t="s">
-        <v>2493</v>
+        <v>2479</v>
       </c>
       <c r="D952" s="35"/>
       <c r="E952" s="27" t="s">
@@ -37123,7 +37053,7 @@
         <v>1106</v>
       </c>
       <c r="C1004" s="31" t="s">
-        <v>2494</v>
+        <v>2480</v>
       </c>
       <c r="D1004" s="27"/>
       <c r="E1004" s="27" t="s">
@@ -37139,7 +37069,7 @@
         <v>17</v>
       </c>
       <c r="I1004" s="29" t="s">
-        <v>2499</v>
+        <v>2485</v>
       </c>
       <c r="J1004" s="27"/>
       <c r="K1004" s="27"/>
@@ -37962,7 +37892,7 @@
         <v>1106</v>
       </c>
       <c r="C1035" s="31" t="s">
-        <v>2500</v>
+        <v>2486</v>
       </c>
       <c r="D1035" s="27"/>
       <c r="E1035" s="27" t="s">
@@ -38315,7 +38245,7 @@
         <v>1106</v>
       </c>
       <c r="C1048" s="31" t="s">
-        <v>2501</v>
+        <v>2487</v>
       </c>
       <c r="D1048" s="27"/>
       <c r="E1048" s="27" t="s">
@@ -38371,7 +38301,7 @@
         <v>1106</v>
       </c>
       <c r="C1050" s="31" t="s">
-        <v>2502</v>
+        <v>2488</v>
       </c>
       <c r="D1050" s="27"/>
       <c r="E1050" s="27" t="s">
@@ -39389,7 +39319,7 @@
       <c r="J1087" s="27"/>
       <c r="K1087" s="27"/>
     </row>
-    <row r="1088" spans="1:11" s="24" customFormat="1" ht="45">
+    <row r="1088" spans="1:11" s="24" customFormat="1" ht="30">
       <c r="A1088" s="51" t="s">
         <v>2396</v>
       </c>
@@ -39412,15 +39342,13 @@
         <v>15</v>
       </c>
       <c r="H1088" s="46" t="s">
-        <v>20</v>
-      </c>
-      <c r="I1088" s="42" t="s">
-        <v>2317</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="I1088" s="42"/>
       <c r="J1088" s="27"/>
       <c r="K1088" s="27"/>
     </row>
-    <row r="1089" spans="1:11" s="24" customFormat="1" ht="45">
+    <row r="1089" spans="1:11" s="24" customFormat="1" ht="30">
       <c r="A1089" s="51" t="s">
         <v>2397</v>
       </c>
@@ -39443,15 +39371,13 @@
         <v>15</v>
       </c>
       <c r="H1089" s="46" t="s">
-        <v>20</v>
-      </c>
-      <c r="I1089" s="48" t="s">
-        <v>2317</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="I1089" s="48"/>
       <c r="J1089" s="27"/>
       <c r="K1089" s="27"/>
     </row>
-    <row r="1090" spans="1:11" s="24" customFormat="1" ht="45">
+    <row r="1090" spans="1:11" s="24" customFormat="1" ht="30">
       <c r="A1090" s="51" t="s">
         <v>2398</v>
       </c>
@@ -39474,15 +39400,13 @@
         <v>15</v>
       </c>
       <c r="H1090" s="46" t="s">
-        <v>20</v>
-      </c>
-      <c r="I1090" s="48" t="s">
-        <v>2317</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="I1090" s="48"/>
       <c r="J1090" s="27"/>
       <c r="K1090" s="27"/>
     </row>
-    <row r="1091" spans="1:11" s="24" customFormat="1" ht="45">
+    <row r="1091" spans="1:11" s="24" customFormat="1" ht="30">
       <c r="A1091" s="51" t="s">
         <v>2399</v>
       </c>
@@ -39505,15 +39429,13 @@
         <v>15</v>
       </c>
       <c r="H1091" s="46" t="s">
-        <v>20</v>
-      </c>
-      <c r="I1091" s="48" t="s">
-        <v>2317</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="I1091" s="48"/>
       <c r="J1091" s="27"/>
       <c r="K1091" s="27"/>
     </row>
-    <row r="1092" spans="1:11" s="24" customFormat="1" ht="45">
+    <row r="1092" spans="1:11" s="24" customFormat="1" ht="30">
       <c r="A1092" s="51" t="s">
         <v>2400</v>
       </c>
@@ -39536,15 +39458,13 @@
         <v>15</v>
       </c>
       <c r="H1092" s="46" t="s">
-        <v>20</v>
-      </c>
-      <c r="I1092" s="48" t="s">
-        <v>2317</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="I1092" s="48"/>
       <c r="J1092" s="27"/>
       <c r="K1092" s="27"/>
     </row>
-    <row r="1093" spans="1:11" s="24" customFormat="1" ht="45">
+    <row r="1093" spans="1:11" s="24" customFormat="1" ht="30">
       <c r="A1093" s="51" t="s">
         <v>2401</v>
       </c>
@@ -39567,15 +39487,13 @@
         <v>15</v>
       </c>
       <c r="H1093" s="46" t="s">
-        <v>20</v>
-      </c>
-      <c r="I1093" s="48" t="s">
-        <v>2317</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="I1093" s="48"/>
       <c r="J1093" s="27"/>
       <c r="K1093" s="27"/>
     </row>
-    <row r="1094" spans="1:11" s="24" customFormat="1" ht="45">
+    <row r="1094" spans="1:11" s="24" customFormat="1" ht="30">
       <c r="A1094" s="51" t="s">
         <v>2402</v>
       </c>
@@ -39598,26 +39516,24 @@
         <v>15</v>
       </c>
       <c r="H1094" s="46" t="s">
-        <v>20</v>
-      </c>
-      <c r="I1094" s="48" t="s">
-        <v>2317</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="I1094" s="48"/>
       <c r="J1094" s="27"/>
       <c r="K1094" s="27"/>
     </row>
-    <row r="1095" spans="1:11" s="24" customFormat="1" ht="45">
+    <row r="1095" spans="1:11" s="24" customFormat="1" ht="30">
       <c r="A1095" s="51" t="s">
-        <v>2438</v>
+        <v>2431</v>
       </c>
       <c r="B1095" s="47">
         <v>7</v>
       </c>
       <c r="C1095" s="42" t="s">
-        <v>2445</v>
+        <v>2438</v>
       </c>
       <c r="D1095" s="51" t="s">
-        <v>2431</v>
+        <v>2424</v>
       </c>
       <c r="E1095" s="27" t="s">
         <v>22</v>
@@ -39629,26 +39545,24 @@
         <v>15</v>
       </c>
       <c r="H1095" s="46" t="s">
-        <v>20</v>
-      </c>
-      <c r="I1095" s="48" t="s">
-        <v>2317</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="I1095" s="48"/>
       <c r="J1095" s="27"/>
       <c r="K1095" s="27"/>
     </row>
-    <row r="1096" spans="1:11" s="24" customFormat="1" ht="45">
+    <row r="1096" spans="1:11" s="24" customFormat="1" ht="30">
       <c r="A1096" s="51" t="s">
-        <v>2439</v>
+        <v>2432</v>
       </c>
       <c r="B1096" s="47">
         <v>7</v>
       </c>
       <c r="C1096" s="42" t="s">
-        <v>2446</v>
+        <v>2439</v>
       </c>
       <c r="D1096" s="51" t="s">
-        <v>2432</v>
+        <v>2425</v>
       </c>
       <c r="E1096" s="27" t="s">
         <v>22</v>
@@ -39660,26 +39574,24 @@
         <v>15</v>
       </c>
       <c r="H1096" s="46" t="s">
-        <v>20</v>
-      </c>
-      <c r="I1096" s="48" t="s">
-        <v>2317</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="I1096" s="48"/>
       <c r="J1096" s="27"/>
       <c r="K1096" s="27"/>
     </row>
-    <row r="1097" spans="1:11" s="24" customFormat="1" ht="45">
+    <row r="1097" spans="1:11" s="24" customFormat="1" ht="30">
       <c r="A1097" s="51" t="s">
-        <v>2440</v>
+        <v>2433</v>
       </c>
       <c r="B1097" s="47">
         <v>7</v>
       </c>
       <c r="C1097" s="42" t="s">
-        <v>2447</v>
+        <v>2440</v>
       </c>
       <c r="D1097" s="51" t="s">
-        <v>2433</v>
+        <v>2426</v>
       </c>
       <c r="E1097" s="27" t="s">
         <v>22</v>
@@ -39691,26 +39603,24 @@
         <v>15</v>
       </c>
       <c r="H1097" s="46" t="s">
-        <v>20</v>
-      </c>
-      <c r="I1097" s="48" t="s">
-        <v>2317</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="I1097" s="48"/>
       <c r="J1097" s="27"/>
       <c r="K1097" s="27"/>
     </row>
-    <row r="1098" spans="1:11" s="24" customFormat="1" ht="45">
+    <row r="1098" spans="1:11" s="24" customFormat="1" ht="30">
       <c r="A1098" s="51" t="s">
-        <v>2441</v>
+        <v>2434</v>
       </c>
       <c r="B1098" s="47">
         <v>7</v>
       </c>
       <c r="C1098" s="42" t="s">
-        <v>2448</v>
+        <v>2441</v>
       </c>
       <c r="D1098" s="51" t="s">
-        <v>2434</v>
+        <v>2427</v>
       </c>
       <c r="E1098" s="27" t="s">
         <v>22</v>
@@ -39722,26 +39632,24 @@
         <v>15</v>
       </c>
       <c r="H1098" s="46" t="s">
-        <v>20</v>
-      </c>
-      <c r="I1098" s="48" t="s">
-        <v>2317</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="I1098" s="48"/>
       <c r="J1098" s="27"/>
       <c r="K1098" s="27"/>
     </row>
-    <row r="1099" spans="1:11" s="24" customFormat="1" ht="45">
+    <row r="1099" spans="1:11" s="24" customFormat="1" ht="30">
       <c r="A1099" s="51" t="s">
-        <v>2442</v>
+        <v>2435</v>
       </c>
       <c r="B1099" s="47">
         <v>7</v>
       </c>
       <c r="C1099" s="42" t="s">
-        <v>2449</v>
+        <v>2442</v>
       </c>
       <c r="D1099" s="51" t="s">
-        <v>2435</v>
+        <v>2428</v>
       </c>
       <c r="E1099" s="27" t="s">
         <v>22</v>
@@ -39753,26 +39661,24 @@
         <v>15</v>
       </c>
       <c r="H1099" s="46" t="s">
-        <v>20</v>
-      </c>
-      <c r="I1099" s="48" t="s">
-        <v>2317</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="I1099" s="48"/>
       <c r="J1099" s="27"/>
       <c r="K1099" s="27"/>
     </row>
-    <row r="1100" spans="1:11" s="24" customFormat="1" ht="45">
+    <row r="1100" spans="1:11" s="24" customFormat="1" ht="30">
       <c r="A1100" s="51" t="s">
-        <v>2443</v>
+        <v>2436</v>
       </c>
       <c r="B1100" s="47">
         <v>7</v>
       </c>
       <c r="C1100" s="42" t="s">
-        <v>2450</v>
+        <v>2443</v>
       </c>
       <c r="D1100" s="51" t="s">
-        <v>2436</v>
+        <v>2429</v>
       </c>
       <c r="E1100" s="27" t="s">
         <v>22</v>
@@ -39784,26 +39690,24 @@
         <v>15</v>
       </c>
       <c r="H1100" s="46" t="s">
-        <v>20</v>
-      </c>
-      <c r="I1100" s="48" t="s">
-        <v>2317</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="I1100" s="48"/>
       <c r="J1100" s="27"/>
       <c r="K1100" s="27"/>
     </row>
-    <row r="1101" spans="1:11" s="24" customFormat="1" ht="45">
+    <row r="1101" spans="1:11" s="24" customFormat="1" ht="30">
       <c r="A1101" s="51" t="s">
-        <v>2444</v>
+        <v>2437</v>
       </c>
       <c r="B1101" s="47">
         <v>7</v>
       </c>
       <c r="C1101" s="42" t="s">
-        <v>2451</v>
+        <v>2444</v>
       </c>
       <c r="D1101" s="51" t="s">
-        <v>2437</v>
+        <v>2430</v>
       </c>
       <c r="E1101" s="27" t="s">
         <v>22</v>
@@ -39815,26 +39719,24 @@
         <v>15</v>
       </c>
       <c r="H1101" s="46" t="s">
-        <v>20</v>
-      </c>
-      <c r="I1101" s="48" t="s">
-        <v>2317</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="I1101" s="48"/>
       <c r="J1101" s="27"/>
       <c r="K1101" s="27"/>
     </row>
     <row r="1102" spans="1:11" s="24" customFormat="1" ht="45">
       <c r="A1102" s="51" t="s">
-        <v>2464</v>
+        <v>2450</v>
       </c>
       <c r="B1102" s="47">
         <v>7</v>
       </c>
       <c r="C1102" s="42" t="s">
-        <v>2465</v>
+        <v>2451</v>
       </c>
       <c r="D1102" s="51" t="s">
-        <v>2463</v>
+        <v>2449</v>
       </c>
       <c r="E1102" s="27" t="s">
         <v>22</v>
@@ -40350,7 +40252,7 @@
         <v>7</v>
       </c>
       <c r="C1119" s="31" t="s">
-        <v>2503</v>
+        <v>2489</v>
       </c>
       <c r="D1119" s="27"/>
       <c r="E1119" s="27" t="s">
@@ -40686,7 +40588,7 @@
         <v>7</v>
       </c>
       <c r="C1131" s="31" t="s">
-        <v>2504</v>
+        <v>2490</v>
       </c>
       <c r="D1131" s="27" t="s">
         <v>2149</v>
@@ -40717,7 +40619,7 @@
         <v>7</v>
       </c>
       <c r="C1132" s="31" t="s">
-        <v>2505</v>
+        <v>2491</v>
       </c>
       <c r="D1132" s="27"/>
       <c r="E1132" s="27" t="s">
@@ -41305,16 +41207,16 @@
     </row>
     <row r="1154" spans="1:11" s="24" customFormat="1" ht="45">
       <c r="A1154" s="51" t="s">
-        <v>2483</v>
+        <v>2469</v>
       </c>
       <c r="B1154" s="47">
         <v>7</v>
       </c>
       <c r="C1154" s="42" t="s">
-        <v>2486</v>
+        <v>2472</v>
       </c>
       <c r="D1154" s="51" t="s">
-        <v>2485</v>
+        <v>2471</v>
       </c>
       <c r="E1154" s="27" t="s">
         <v>22</v>
@@ -41334,16 +41236,16 @@
     </row>
     <row r="1155" spans="1:11" s="24" customFormat="1" ht="45">
       <c r="A1155" s="51" t="s">
-        <v>2484</v>
+        <v>2470</v>
       </c>
       <c r="B1155" s="47">
         <v>7</v>
       </c>
       <c r="C1155" s="42" t="s">
-        <v>2487</v>
+        <v>2473</v>
       </c>
       <c r="D1155" s="51" t="s">
-        <v>2485</v>
+        <v>2471</v>
       </c>
       <c r="E1155" s="27" t="s">
         <v>22</v>
@@ -41776,7 +41678,7 @@
         <v>7</v>
       </c>
       <c r="C1171" s="31" t="s">
-        <v>2506</v>
+        <v>2492</v>
       </c>
       <c r="D1171" s="27"/>
       <c r="E1171" s="27" t="s">
@@ -41797,13 +41699,13 @@
     </row>
     <row r="1172" spans="1:11" s="24" customFormat="1" ht="45">
       <c r="A1172" s="51" t="s">
-        <v>2495</v>
+        <v>2481</v>
       </c>
       <c r="B1172" s="47">
         <v>7</v>
       </c>
       <c r="C1172" s="42" t="s">
-        <v>2497</v>
+        <v>2483</v>
       </c>
       <c r="D1172" s="46"/>
       <c r="E1172" s="27" t="s">
@@ -41826,13 +41728,13 @@
     </row>
     <row r="1173" spans="1:11" s="24" customFormat="1" ht="45">
       <c r="A1173" s="51" t="s">
-        <v>2496</v>
+        <v>2482</v>
       </c>
       <c r="B1173" s="47">
         <v>7</v>
       </c>
       <c r="C1173" s="42" t="s">
-        <v>2498</v>
+        <v>2484</v>
       </c>
       <c r="D1173" s="46"/>
       <c r="E1173" s="27" t="s">
@@ -41861,7 +41763,7 @@
         <v>7</v>
       </c>
       <c r="C1174" s="31" t="s">
-        <v>2507</v>
+        <v>2493</v>
       </c>
       <c r="D1174" s="27"/>
       <c r="E1174" s="27" t="s">
@@ -42488,6 +42390,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F2EA47BB262D974097182E2CA8AB13E1" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="74597e8d9e42e7e4fc8eda6d37675aa2">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4aeb20c0e3442673af7ee10786458764">
     <xsd:element name="properties">
@@ -42536,37 +42453,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EDB2DE12-5EF6-4CF2-820D-5F9FE329E08E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/internal/2005/internalDocumentation"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{923F65C5-DEAB-400B-AA1F-124F40EE10AC}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
@@ -42580,10 +42467,25 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6D33261-F3C6-4621-88F1-D76E5ABE1865}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EDB2DE12-5EF6-4CF2-820D-5F9FE329E08E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/internal/2005/internalDocumentation"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
[MS-OUTSPS]: Add new cases and capture code for 5 fixed TDIs\TDQs
</commit_message>
<xml_diff>
--- a/SharePoint/Docs/MS-OUTSPS/MS-OUTSPS_RequirementSpecification.xlsx
+++ b/SharePoint/Docs/MS-OUTSPS/MS-OUTSPS_RequirementSpecification.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8118" uniqueCount="2495">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8116" uniqueCount="2494">
   <si>
     <t>Req ID</t>
   </si>
@@ -7001,9 +7001,6 @@
   </si>
   <si>
     <t>[In Message Processing Events and Sequencing Rules][The operation]GetList &lt;2&gt; Gets information about a list.</t>
-  </si>
-  <si>
-    <t>[In Common Schema]Unless stated otherwise[Categories, Modified, ReplicationID], all fields in this section[Attachments, ContentTypeId, Created, ID, owshiddenversion, ReplicationID, vti_versionhistory] MUST be present on all item types&lt;20&gt; and contain valid data.</t>
   </si>
   <si>
     <t>[In Contact-Specific Schema][One of the contact properties appears as the attributes of the element GetListResponse.GetListResult.List.Fields.Field. Field.Name:]Account[ Field.ID:]None defined[Field.Type:]None defined (Text).</t>
@@ -8014,9 +8011,6 @@
     <t>[In Appendix B: Product Behavior] Implementation does default the value of AllDayEvent to 0 which means false if fAllDayEvent is empty or missing. (Windows SharePoint Services 3.0 and above follow this behavior.)</t>
   </si>
   <si>
-    <t>Verified by derived requirement: MS-OUTSPS_R2812.</t>
-  </si>
-  <si>
     <t>[In Appointment-Specific Schema][For fRecurrence]1 means it[event] is a recurring event or an exception,</t>
   </si>
   <si>
@@ -8095,6 +8089,9 @@
   </si>
   <si>
     <t>[In Contacts]Contacts have some information about a person, group, business, or other entity.</t>
+  </si>
+  <si>
+    <t>[In Common Schema]Unless stated otherwise[Attachments, Categories, Created, Modified, ReplicationID, vti_versionhistory], all fields in this section[ContentTypeId, ID, owshiddenversion] MUST be present on all item types&lt;20&gt; and contain valid data.</t>
   </si>
 </sst>
 </file>
@@ -10151,7 +10148,7 @@
     </row>
     <row r="2" spans="1:9">
       <c r="A2" s="5" t="s">
-        <v>2330</v>
+        <v>2329</v>
       </c>
       <c r="B2" s="6"/>
       <c r="C2" s="6"/>
@@ -10164,10 +10161,10 @@
         <v>25</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>2331</v>
+        <v>2330</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>2329</v>
+        <v>2328</v>
       </c>
       <c r="F3" s="12">
         <v>42566</v>
@@ -10433,13 +10430,13 @@
     </row>
     <row r="20" spans="1:11" ht="30">
       <c r="A20" s="46" t="s">
-        <v>2332</v>
+        <v>2331</v>
       </c>
       <c r="B20" s="47">
         <v>2</v>
       </c>
       <c r="C20" s="42" t="s">
-        <v>2335</v>
+        <v>2334</v>
       </c>
       <c r="D20" s="46"/>
       <c r="E20" s="46" t="s">
@@ -10458,13 +10455,13 @@
     </row>
     <row r="21" spans="1:11" ht="30">
       <c r="A21" s="46" t="s">
-        <v>2333</v>
+        <v>2332</v>
       </c>
       <c r="B21" s="47">
         <v>2</v>
       </c>
       <c r="C21" s="42" t="s">
-        <v>2336</v>
+        <v>2335</v>
       </c>
       <c r="D21" s="46"/>
       <c r="E21" s="46" t="s">
@@ -10483,13 +10480,13 @@
     </row>
     <row r="22" spans="1:11" ht="30">
       <c r="A22" s="46" t="s">
-        <v>2334</v>
+        <v>2333</v>
       </c>
       <c r="B22" s="47">
         <v>2</v>
       </c>
       <c r="C22" s="42" t="s">
-        <v>2337</v>
+        <v>2336</v>
       </c>
       <c r="D22" s="46"/>
       <c r="E22" s="46" t="s">
@@ -10508,13 +10505,13 @@
     </row>
     <row r="23" spans="1:11" ht="45">
       <c r="A23" s="46" t="s">
-        <v>2338</v>
+        <v>2337</v>
       </c>
       <c r="B23" s="47">
         <v>2</v>
       </c>
       <c r="C23" s="42" t="s">
-        <v>2339</v>
+        <v>2338</v>
       </c>
       <c r="D23" s="46"/>
       <c r="E23" s="46" t="s">
@@ -11054,7 +11051,7 @@
         <v>63</v>
       </c>
       <c r="C43" s="31" t="s">
-        <v>2340</v>
+        <v>2339</v>
       </c>
       <c r="D43" s="27"/>
       <c r="E43" s="27" t="s">
@@ -11151,7 +11148,7 @@
         <v>17</v>
       </c>
       <c r="I46" s="29" t="s">
-        <v>2263</v>
+        <v>2262</v>
       </c>
       <c r="J46" s="27"/>
       <c r="K46" s="27"/>
@@ -11209,7 +11206,7 @@
         <v>17</v>
       </c>
       <c r="I48" s="29" t="s">
-        <v>2264</v>
+        <v>2263</v>
       </c>
       <c r="J48" s="27"/>
       <c r="K48" s="27"/>
@@ -11267,7 +11264,7 @@
         <v>17</v>
       </c>
       <c r="I50" s="29" t="s">
-        <v>2265</v>
+        <v>2264</v>
       </c>
       <c r="J50" s="27"/>
       <c r="K50" s="27"/>
@@ -11309,7 +11306,7 @@
         <v>81</v>
       </c>
       <c r="C52" s="31" t="s">
-        <v>2341</v>
+        <v>2340</v>
       </c>
       <c r="D52" s="27"/>
       <c r="E52" s="27" t="s">
@@ -11363,7 +11360,7 @@
         <v>85</v>
       </c>
       <c r="C54" s="31" t="s">
-        <v>2342</v>
+        <v>2341</v>
       </c>
       <c r="D54" s="27"/>
       <c r="E54" s="27" t="s">
@@ -11444,7 +11441,7 @@
         <v>91</v>
       </c>
       <c r="C57" s="31" t="s">
-        <v>2343</v>
+        <v>2342</v>
       </c>
       <c r="D57" s="27"/>
       <c r="E57" s="27" t="s">
@@ -11492,13 +11489,13 @@
     </row>
     <row r="59" spans="1:11" s="24" customFormat="1" ht="30">
       <c r="A59" s="46" t="s">
-        <v>2344</v>
+        <v>2343</v>
       </c>
       <c r="B59" s="47" t="s">
         <v>91</v>
       </c>
       <c r="C59" s="42" t="s">
-        <v>2350</v>
+        <v>2349</v>
       </c>
       <c r="D59" s="46"/>
       <c r="E59" s="46" t="s">
@@ -11519,13 +11516,13 @@
     </row>
     <row r="60" spans="1:11" s="24" customFormat="1" ht="30">
       <c r="A60" s="46" t="s">
-        <v>2345</v>
+        <v>2344</v>
       </c>
       <c r="B60" s="47" t="s">
         <v>91</v>
       </c>
       <c r="C60" s="42" t="s">
-        <v>2351</v>
+        <v>2350</v>
       </c>
       <c r="D60" s="46"/>
       <c r="E60" s="46" t="s">
@@ -11546,13 +11543,13 @@
     </row>
     <row r="61" spans="1:11" s="24" customFormat="1">
       <c r="A61" s="46" t="s">
-        <v>2346</v>
+        <v>2345</v>
       </c>
       <c r="B61" s="47" t="s">
         <v>91</v>
       </c>
       <c r="C61" s="42" t="s">
-        <v>2352</v>
+        <v>2351</v>
       </c>
       <c r="D61" s="46"/>
       <c r="E61" s="46" t="s">
@@ -11573,13 +11570,13 @@
     </row>
     <row r="62" spans="1:11" s="24" customFormat="1">
       <c r="A62" s="46" t="s">
-        <v>2347</v>
+        <v>2346</v>
       </c>
       <c r="B62" s="47" t="s">
         <v>91</v>
       </c>
       <c r="C62" s="42" t="s">
-        <v>2353</v>
+        <v>2352</v>
       </c>
       <c r="D62" s="46"/>
       <c r="E62" s="46" t="s">
@@ -11600,13 +11597,13 @@
     </row>
     <row r="63" spans="1:11" s="24" customFormat="1">
       <c r="A63" s="46" t="s">
-        <v>2348</v>
+        <v>2347</v>
       </c>
       <c r="B63" s="47" t="s">
         <v>91</v>
       </c>
       <c r="C63" s="42" t="s">
-        <v>2354</v>
+        <v>2353</v>
       </c>
       <c r="D63" s="46"/>
       <c r="E63" s="46" t="s">
@@ -11627,13 +11624,13 @@
     </row>
     <row r="64" spans="1:11" s="24" customFormat="1">
       <c r="A64" s="46" t="s">
-        <v>2349</v>
+        <v>2348</v>
       </c>
       <c r="B64" s="43" t="s">
         <v>91</v>
       </c>
       <c r="C64" s="42" t="s">
-        <v>2355</v>
+        <v>2354</v>
       </c>
       <c r="D64" s="46"/>
       <c r="E64" s="46" t="s">
@@ -11654,13 +11651,13 @@
     </row>
     <row r="65" spans="1:11" s="24" customFormat="1" ht="30">
       <c r="A65" s="51" t="s">
-        <v>2357</v>
+        <v>2356</v>
       </c>
       <c r="B65" s="47" t="s">
         <v>91</v>
       </c>
       <c r="C65" s="42" t="s">
-        <v>2356</v>
+        <v>2355</v>
       </c>
       <c r="D65" s="46"/>
       <c r="E65" s="46" t="s">
@@ -11687,7 +11684,7 @@
         <v>91</v>
       </c>
       <c r="C66" s="31" t="s">
-        <v>2358</v>
+        <v>2357</v>
       </c>
       <c r="D66" s="27"/>
       <c r="E66" s="27" t="s">
@@ -11708,13 +11705,13 @@
     </row>
     <row r="67" spans="1:11" s="24" customFormat="1" ht="30">
       <c r="A67" s="51" t="s">
-        <v>2365</v>
+        <v>2364</v>
       </c>
       <c r="B67" s="47" t="s">
         <v>91</v>
       </c>
       <c r="C67" s="31" t="s">
-        <v>2372</v>
+        <v>2371</v>
       </c>
       <c r="D67" s="46"/>
       <c r="E67" s="27" t="s">
@@ -11741,7 +11738,7 @@
         <v>91</v>
       </c>
       <c r="C68" s="31" t="s">
-        <v>2364</v>
+        <v>2363</v>
       </c>
       <c r="D68" s="27"/>
       <c r="E68" s="27" t="s">
@@ -11762,13 +11759,13 @@
     </row>
     <row r="69" spans="1:11" s="24" customFormat="1" ht="30">
       <c r="A69" s="51" t="s">
-        <v>2366</v>
+        <v>2365</v>
       </c>
       <c r="B69" s="47" t="s">
         <v>91</v>
       </c>
       <c r="C69" s="31" t="s">
-        <v>2373</v>
+        <v>2372</v>
       </c>
       <c r="D69" s="46"/>
       <c r="E69" s="27" t="s">
@@ -11795,7 +11792,7 @@
         <v>91</v>
       </c>
       <c r="C70" s="31" t="s">
-        <v>2363</v>
+        <v>2362</v>
       </c>
       <c r="D70" s="27"/>
       <c r="E70" s="27" t="s">
@@ -11816,13 +11813,13 @@
     </row>
     <row r="71" spans="1:11" s="24" customFormat="1" ht="30">
       <c r="A71" s="51" t="s">
-        <v>2367</v>
+        <v>2366</v>
       </c>
       <c r="B71" s="47" t="s">
         <v>91</v>
       </c>
       <c r="C71" s="31" t="s">
-        <v>2374</v>
+        <v>2373</v>
       </c>
       <c r="D71" s="46"/>
       <c r="E71" s="27" t="s">
@@ -11849,7 +11846,7 @@
         <v>91</v>
       </c>
       <c r="C72" s="31" t="s">
-        <v>2362</v>
+        <v>2361</v>
       </c>
       <c r="D72" s="27"/>
       <c r="E72" s="27" t="s">
@@ -11870,13 +11867,13 @@
     </row>
     <row r="73" spans="1:11" s="24" customFormat="1" ht="30">
       <c r="A73" s="51" t="s">
-        <v>2368</v>
+        <v>2367</v>
       </c>
       <c r="B73" s="47" t="s">
         <v>91</v>
       </c>
       <c r="C73" s="42" t="s">
-        <v>2375</v>
+        <v>2374</v>
       </c>
       <c r="D73" s="46"/>
       <c r="E73" s="27" t="s">
@@ -11903,7 +11900,7 @@
         <v>91</v>
       </c>
       <c r="C74" s="31" t="s">
-        <v>2361</v>
+        <v>2360</v>
       </c>
       <c r="D74" s="27"/>
       <c r="E74" s="27" t="s">
@@ -11924,13 +11921,13 @@
     </row>
     <row r="75" spans="1:11" s="24" customFormat="1" ht="30">
       <c r="A75" s="51" t="s">
-        <v>2369</v>
+        <v>2368</v>
       </c>
       <c r="B75" s="47" t="s">
         <v>91</v>
       </c>
       <c r="C75" s="31" t="s">
-        <v>2376</v>
+        <v>2375</v>
       </c>
       <c r="D75" s="46"/>
       <c r="E75" s="27" t="s">
@@ -11957,7 +11954,7 @@
         <v>91</v>
       </c>
       <c r="C76" s="31" t="s">
-        <v>2360</v>
+        <v>2359</v>
       </c>
       <c r="D76" s="27"/>
       <c r="E76" s="27" t="s">
@@ -11978,13 +11975,13 @@
     </row>
     <row r="77" spans="1:11" s="24" customFormat="1" ht="30">
       <c r="A77" s="51" t="s">
-        <v>2370</v>
+        <v>2369</v>
       </c>
       <c r="B77" s="47" t="s">
         <v>91</v>
       </c>
       <c r="C77" s="31" t="s">
-        <v>2377</v>
+        <v>2376</v>
       </c>
       <c r="D77" s="46"/>
       <c r="E77" s="27" t="s">
@@ -12011,7 +12008,7 @@
         <v>91</v>
       </c>
       <c r="C78" s="31" t="s">
-        <v>2359</v>
+        <v>2358</v>
       </c>
       <c r="D78" s="27"/>
       <c r="E78" s="27" t="s">
@@ -12032,13 +12029,13 @@
     </row>
     <row r="79" spans="1:11" s="24" customFormat="1" ht="30">
       <c r="A79" s="51" t="s">
-        <v>2371</v>
+        <v>2370</v>
       </c>
       <c r="B79" s="43" t="s">
         <v>91</v>
       </c>
       <c r="C79" s="31" t="s">
-        <v>2378</v>
+        <v>2377</v>
       </c>
       <c r="D79" s="46"/>
       <c r="E79" s="27" t="s">
@@ -12059,13 +12056,13 @@
     </row>
     <row r="80" spans="1:11" s="24" customFormat="1" ht="30">
       <c r="A80" s="51" t="s">
-        <v>2379</v>
+        <v>2378</v>
       </c>
       <c r="B80" s="47" t="s">
         <v>91</v>
       </c>
       <c r="C80" s="42" t="s">
-        <v>2384</v>
+        <v>2383</v>
       </c>
       <c r="D80" s="46"/>
       <c r="E80" s="27" t="s">
@@ -12086,13 +12083,13 @@
     </row>
     <row r="81" spans="1:11" s="24" customFormat="1">
       <c r="A81" s="51" t="s">
-        <v>2380</v>
+        <v>2379</v>
       </c>
       <c r="B81" s="47" t="s">
         <v>91</v>
       </c>
       <c r="C81" s="42" t="s">
-        <v>2385</v>
+        <v>2384</v>
       </c>
       <c r="D81" s="46"/>
       <c r="E81" s="27" t="s">
@@ -12113,13 +12110,13 @@
     </row>
     <row r="82" spans="1:11" s="24" customFormat="1">
       <c r="A82" s="51" t="s">
-        <v>2381</v>
+        <v>2380</v>
       </c>
       <c r="B82" s="47" t="s">
         <v>91</v>
       </c>
       <c r="C82" s="42" t="s">
-        <v>2386</v>
+        <v>2385</v>
       </c>
       <c r="D82" s="46"/>
       <c r="E82" s="27" t="s">
@@ -12140,13 +12137,13 @@
     </row>
     <row r="83" spans="1:11" s="24" customFormat="1">
       <c r="A83" s="51" t="s">
-        <v>2382</v>
+        <v>2381</v>
       </c>
       <c r="B83" s="47" t="s">
         <v>91</v>
       </c>
       <c r="C83" s="42" t="s">
-        <v>2387</v>
+        <v>2386</v>
       </c>
       <c r="D83" s="46"/>
       <c r="E83" s="27" t="s">
@@ -12167,13 +12164,13 @@
     </row>
     <row r="84" spans="1:11" s="24" customFormat="1">
       <c r="A84" s="51" t="s">
-        <v>2383</v>
+        <v>2382</v>
       </c>
       <c r="B84" s="47" t="s">
         <v>91</v>
       </c>
       <c r="C84" s="42" t="s">
-        <v>2388</v>
+        <v>2387</v>
       </c>
       <c r="D84" s="46"/>
       <c r="E84" s="27" t="s">
@@ -12248,13 +12245,13 @@
     </row>
     <row r="87" spans="1:11" s="24" customFormat="1" ht="30">
       <c r="A87" s="51" t="s">
-        <v>2410</v>
+        <v>2409</v>
       </c>
       <c r="B87" s="47" t="s">
         <v>91</v>
       </c>
       <c r="C87" s="31" t="s">
-        <v>2417</v>
+        <v>2416</v>
       </c>
       <c r="D87" s="46"/>
       <c r="E87" s="27" t="s">
@@ -12302,13 +12299,13 @@
     </row>
     <row r="89" spans="1:11" s="24" customFormat="1" ht="30">
       <c r="A89" s="51" t="s">
-        <v>2411</v>
+        <v>2410</v>
       </c>
       <c r="B89" s="47" t="s">
         <v>91</v>
       </c>
       <c r="C89" s="31" t="s">
-        <v>2418</v>
+        <v>2417</v>
       </c>
       <c r="D89" s="46"/>
       <c r="E89" s="27" t="s">
@@ -12356,13 +12353,13 @@
     </row>
     <row r="91" spans="1:11" s="24" customFormat="1" ht="30">
       <c r="A91" s="51" t="s">
-        <v>2412</v>
+        <v>2411</v>
       </c>
       <c r="B91" s="47" t="s">
         <v>91</v>
       </c>
       <c r="C91" s="31" t="s">
-        <v>2419</v>
+        <v>2418</v>
       </c>
       <c r="D91" s="46"/>
       <c r="E91" s="27" t="s">
@@ -12410,13 +12407,13 @@
     </row>
     <row r="93" spans="1:11" s="24" customFormat="1" ht="30">
       <c r="A93" s="51" t="s">
-        <v>2413</v>
+        <v>2412</v>
       </c>
       <c r="B93" s="47" t="s">
         <v>91</v>
       </c>
       <c r="C93" s="31" t="s">
-        <v>2420</v>
+        <v>2419</v>
       </c>
       <c r="D93" s="46"/>
       <c r="E93" s="27" t="s">
@@ -12464,13 +12461,13 @@
     </row>
     <row r="95" spans="1:11" s="24" customFormat="1" ht="30">
       <c r="A95" s="51" t="s">
-        <v>2414</v>
+        <v>2413</v>
       </c>
       <c r="B95" s="47" t="s">
         <v>91</v>
       </c>
       <c r="C95" s="31" t="s">
-        <v>2421</v>
+        <v>2420</v>
       </c>
       <c r="D95" s="46"/>
       <c r="E95" s="27" t="s">
@@ -12518,13 +12515,13 @@
     </row>
     <row r="97" spans="1:11" s="24" customFormat="1" ht="30">
       <c r="A97" s="51" t="s">
-        <v>2415</v>
+        <v>2414</v>
       </c>
       <c r="B97" s="47" t="s">
         <v>91</v>
       </c>
       <c r="C97" s="31" t="s">
-        <v>2422</v>
+        <v>2421</v>
       </c>
       <c r="D97" s="46"/>
       <c r="E97" s="27" t="s">
@@ -12572,13 +12569,13 @@
     </row>
     <row r="99" spans="1:11" s="24" customFormat="1" ht="30">
       <c r="A99" s="51" t="s">
-        <v>2416</v>
+        <v>2415</v>
       </c>
       <c r="B99" s="47" t="s">
         <v>91</v>
       </c>
       <c r="C99" s="31" t="s">
-        <v>2423</v>
+        <v>2422</v>
       </c>
       <c r="D99" s="46"/>
       <c r="E99" s="27" t="s">
@@ -13320,7 +13317,7 @@
         <v>15</v>
       </c>
       <c r="H126" s="27" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I126" s="29"/>
       <c r="J126" s="27"/>
@@ -13442,7 +13439,7 @@
         <v>180</v>
       </c>
       <c r="C131" s="31" t="s">
-        <v>2445</v>
+        <v>2444</v>
       </c>
       <c r="D131" s="27"/>
       <c r="E131" s="27" t="s">
@@ -13455,7 +13452,7 @@
         <v>15</v>
       </c>
       <c r="H131" s="27" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I131" s="29"/>
       <c r="J131" s="27"/>
@@ -13496,7 +13493,7 @@
         <v>183</v>
       </c>
       <c r="C133" s="31" t="s">
-        <v>2446</v>
+        <v>2445</v>
       </c>
       <c r="D133" s="27"/>
       <c r="E133" s="27" t="s">
@@ -13509,7 +13506,7 @@
         <v>15</v>
       </c>
       <c r="H133" s="27" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I133" s="29"/>
       <c r="J133" s="27"/>
@@ -13799,7 +13796,7 @@
         <v>183</v>
       </c>
       <c r="C144" s="31" t="s">
-        <v>2266</v>
+        <v>2265</v>
       </c>
       <c r="D144" s="27" t="s">
         <v>205</v>
@@ -13822,13 +13819,13 @@
     </row>
     <row r="145" spans="1:11" s="24" customFormat="1" ht="30">
       <c r="A145" s="46" t="s">
-        <v>2447</v>
+        <v>2446</v>
       </c>
       <c r="B145" s="47" t="s">
         <v>183</v>
       </c>
       <c r="C145" s="31" t="s">
-        <v>2448</v>
+        <v>2447</v>
       </c>
       <c r="D145" s="46"/>
       <c r="E145" s="46" t="s">
@@ -13844,7 +13841,7 @@
         <v>17</v>
       </c>
       <c r="I145" s="42" t="s">
-        <v>2452</v>
+        <v>2451</v>
       </c>
       <c r="J145" s="27"/>
       <c r="K145" s="27"/>
@@ -15990,7 +15987,7 @@
         <v>298</v>
       </c>
       <c r="C225" s="31" t="s">
-        <v>2267</v>
+        <v>2266</v>
       </c>
       <c r="D225" s="27"/>
       <c r="E225" s="27" t="s">
@@ -16017,7 +16014,7 @@
         <v>298</v>
       </c>
       <c r="C226" s="31" t="s">
-        <v>2268</v>
+        <v>2267</v>
       </c>
       <c r="D226" s="27"/>
       <c r="E226" s="27" t="s">
@@ -16044,7 +16041,7 @@
         <v>298</v>
       </c>
       <c r="C227" s="31" t="s">
-        <v>2269</v>
+        <v>2268</v>
       </c>
       <c r="D227" s="27"/>
       <c r="E227" s="27" t="s">
@@ -16071,7 +16068,7 @@
         <v>298</v>
       </c>
       <c r="C228" s="31" t="s">
-        <v>2315</v>
+        <v>2314</v>
       </c>
       <c r="D228" s="27"/>
       <c r="E228" s="27" t="s">
@@ -16098,7 +16095,7 @@
         <v>298</v>
       </c>
       <c r="C229" s="31" t="s">
-        <v>2270</v>
+        <v>2269</v>
       </c>
       <c r="D229" s="27"/>
       <c r="E229" s="27" t="s">
@@ -16125,7 +16122,7 @@
         <v>298</v>
       </c>
       <c r="C230" s="31" t="s">
-        <v>2271</v>
+        <v>2270</v>
       </c>
       <c r="D230" s="27"/>
       <c r="E230" s="27" t="s">
@@ -16152,7 +16149,7 @@
         <v>298</v>
       </c>
       <c r="C231" s="31" t="s">
-        <v>2272</v>
+        <v>2271</v>
       </c>
       <c r="D231" s="27"/>
       <c r="E231" s="27" t="s">
@@ -16530,7 +16527,7 @@
         <v>319</v>
       </c>
       <c r="C245" s="31" t="s">
-        <v>2453</v>
+        <v>2452</v>
       </c>
       <c r="D245" s="27"/>
       <c r="E245" s="27" t="s">
@@ -16816,7 +16813,7 @@
         <v>17</v>
       </c>
       <c r="I255" s="29" t="s">
-        <v>2323</v>
+        <v>2322</v>
       </c>
       <c r="J255" s="27"/>
       <c r="K255" s="27"/>
@@ -18897,7 +18894,7 @@
         <v>17</v>
       </c>
       <c r="I332" s="29" t="s">
-        <v>2320</v>
+        <v>2319</v>
       </c>
       <c r="J332" s="27"/>
       <c r="K332" s="27"/>
@@ -19153,7 +19150,7 @@
         <v>416</v>
       </c>
       <c r="C342" s="31" t="s">
-        <v>2454</v>
+        <v>2453</v>
       </c>
       <c r="D342" s="27"/>
       <c r="E342" s="27" t="s">
@@ -20665,7 +20662,7 @@
         <v>487</v>
       </c>
       <c r="C398" s="31" t="s">
-        <v>2273</v>
+        <v>2272</v>
       </c>
       <c r="D398" s="27"/>
       <c r="E398" s="27" t="s">
@@ -20692,7 +20689,7 @@
         <v>487</v>
       </c>
       <c r="C399" s="31" t="s">
-        <v>2274</v>
+        <v>2273</v>
       </c>
       <c r="D399" s="27"/>
       <c r="E399" s="27" t="s">
@@ -20719,7 +20716,7 @@
         <v>487</v>
       </c>
       <c r="C400" s="31" t="s">
-        <v>2275</v>
+        <v>2274</v>
       </c>
       <c r="D400" s="27"/>
       <c r="E400" s="27" t="s">
@@ -20746,7 +20743,7 @@
         <v>487</v>
       </c>
       <c r="C401" s="31" t="s">
-        <v>2276</v>
+        <v>2275</v>
       </c>
       <c r="D401" s="27"/>
       <c r="E401" s="27" t="s">
@@ -20773,7 +20770,7 @@
         <v>487</v>
       </c>
       <c r="C402" s="31" t="s">
-        <v>2277</v>
+        <v>2276</v>
       </c>
       <c r="D402" s="27"/>
       <c r="E402" s="27" t="s">
@@ -20800,7 +20797,7 @@
         <v>487</v>
       </c>
       <c r="C403" s="31" t="s">
-        <v>2278</v>
+        <v>2277</v>
       </c>
       <c r="D403" s="27"/>
       <c r="E403" s="27" t="s">
@@ -20827,7 +20824,7 @@
         <v>487</v>
       </c>
       <c r="C404" s="31" t="s">
-        <v>2279</v>
+        <v>2278</v>
       </c>
       <c r="D404" s="27"/>
       <c r="E404" s="27" t="s">
@@ -20854,7 +20851,7 @@
         <v>487</v>
       </c>
       <c r="C405" s="31" t="s">
-        <v>2280</v>
+        <v>2279</v>
       </c>
       <c r="D405" s="27"/>
       <c r="E405" s="27" t="s">
@@ -20881,7 +20878,7 @@
         <v>487</v>
       </c>
       <c r="C406" s="31" t="s">
-        <v>2281</v>
+        <v>2280</v>
       </c>
       <c r="D406" s="27"/>
       <c r="E406" s="27" t="s">
@@ -21259,7 +21256,7 @@
         <v>510</v>
       </c>
       <c r="C420" s="31" t="s">
-        <v>2455</v>
+        <v>2454</v>
       </c>
       <c r="D420" s="27"/>
       <c r="E420" s="27" t="s">
@@ -21475,7 +21472,7 @@
         <v>526</v>
       </c>
       <c r="C428" s="42" t="s">
-        <v>2453</v>
+        <v>2452</v>
       </c>
       <c r="D428" s="35"/>
       <c r="E428" s="27" t="s">
@@ -22168,7 +22165,7 @@
         <v>17</v>
       </c>
       <c r="I453" s="29" t="s">
-        <v>2321</v>
+        <v>2320</v>
       </c>
       <c r="J453" s="27"/>
       <c r="K453" s="27"/>
@@ -22413,7 +22410,7 @@
         <v>17</v>
       </c>
       <c r="I462" s="29" t="s">
-        <v>2316</v>
+        <v>2315</v>
       </c>
       <c r="J462" s="27"/>
       <c r="K462" s="27"/>
@@ -22750,7 +22747,7 @@
         <v>578</v>
       </c>
       <c r="C475" s="31" t="s">
-        <v>2494</v>
+        <v>2492</v>
       </c>
       <c r="D475" s="27"/>
       <c r="E475" s="27" t="s">
@@ -23074,7 +23071,7 @@
         <v>591</v>
       </c>
       <c r="C487" s="31" t="s">
-        <v>2456</v>
+        <v>2455</v>
       </c>
       <c r="D487" s="27"/>
       <c r="E487" s="27" t="s">
@@ -23290,7 +23287,7 @@
         <v>599</v>
       </c>
       <c r="C495" s="31" t="s">
-        <v>2457</v>
+        <v>2456</v>
       </c>
       <c r="D495" s="27"/>
       <c r="E495" s="27" t="s">
@@ -24316,7 +24313,7 @@
         <v>620</v>
       </c>
       <c r="C533" s="31" t="s">
-        <v>2458</v>
+        <v>2457</v>
       </c>
       <c r="D533" s="27"/>
       <c r="E533" s="27" t="s">
@@ -24424,7 +24421,7 @@
         <v>644</v>
       </c>
       <c r="C537" s="31" t="s">
-        <v>2190</v>
+        <v>2493</v>
       </c>
       <c r="D537" s="27"/>
       <c r="E537" s="27" t="s">
@@ -24437,7 +24434,7 @@
         <v>15</v>
       </c>
       <c r="H537" s="27" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I537" s="29"/>
       <c r="J537" s="27"/>
@@ -24715,13 +24712,13 @@
     </row>
     <row r="548" spans="1:11" s="24" customFormat="1">
       <c r="A548" s="51" t="s">
-        <v>2459</v>
+        <v>2458</v>
       </c>
       <c r="B548" s="43" t="s">
         <v>644</v>
       </c>
       <c r="C548" s="31" t="s">
-        <v>2460</v>
+        <v>2459</v>
       </c>
       <c r="D548" s="46"/>
       <c r="E548" s="27" t="s">
@@ -24964,7 +24961,7 @@
         <v>644</v>
       </c>
       <c r="C557" s="31" t="s">
-        <v>2461</v>
+        <v>2460</v>
       </c>
       <c r="D557" s="27"/>
       <c r="E557" s="27" t="s">
@@ -25371,7 +25368,7 @@
         <v>644</v>
       </c>
       <c r="C572" s="31" t="s">
-        <v>2282</v>
+        <v>2281</v>
       </c>
       <c r="D572" s="27" t="s">
         <v>680</v>
@@ -25745,13 +25742,13 @@
     </row>
     <row r="586" spans="1:11" s="24" customFormat="1">
       <c r="A586" s="51" t="s">
-        <v>2462</v>
+        <v>2461</v>
       </c>
       <c r="B586" s="47" t="s">
         <v>644</v>
       </c>
       <c r="C586" s="31" t="s">
-        <v>2463</v>
+        <v>2462</v>
       </c>
       <c r="D586" s="46"/>
       <c r="E586" s="27" t="s">
@@ -25778,7 +25775,7 @@
         <v>644</v>
       </c>
       <c r="C587" s="31" t="s">
-        <v>2283</v>
+        <v>2282</v>
       </c>
       <c r="D587" s="27"/>
       <c r="E587" s="27" t="s">
@@ -26912,7 +26909,7 @@
         <v>706</v>
       </c>
       <c r="C629" s="31" t="s">
-        <v>2464</v>
+        <v>2463</v>
       </c>
       <c r="D629" s="27"/>
       <c r="E629" s="27" t="s">
@@ -26933,13 +26930,13 @@
     </row>
     <row r="630" spans="1:11" s="24" customFormat="1" ht="30">
       <c r="A630" s="51" t="s">
-        <v>2465</v>
+        <v>2464</v>
       </c>
       <c r="B630" s="47" t="s">
         <v>706</v>
       </c>
       <c r="C630" s="31" t="s">
-        <v>2466</v>
+        <v>2465</v>
       </c>
       <c r="D630" s="46"/>
       <c r="E630" s="27" t="s">
@@ -26966,7 +26963,7 @@
         <v>706</v>
       </c>
       <c r="C631" s="31" t="s">
-        <v>2467</v>
+        <v>2466</v>
       </c>
       <c r="D631" s="27"/>
       <c r="E631" s="27" t="s">
@@ -27425,7 +27422,7 @@
         <v>706</v>
       </c>
       <c r="C648" s="31" t="s">
-        <v>2468</v>
+        <v>2467</v>
       </c>
       <c r="D648" s="27"/>
       <c r="E648" s="27" t="s">
@@ -27440,9 +27437,7 @@
       <c r="H648" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="I648" s="29" t="s">
-        <v>2474</v>
-      </c>
+      <c r="I648" s="29"/>
       <c r="J648" s="27"/>
       <c r="K648" s="27"/>
     </row>
@@ -27562,7 +27557,7 @@
         <v>706</v>
       </c>
       <c r="C653" s="31" t="s">
-        <v>2475</v>
+        <v>2473</v>
       </c>
       <c r="D653" s="27"/>
       <c r="E653" s="27" t="s">
@@ -27886,7 +27881,7 @@
         <v>706</v>
       </c>
       <c r="C665" s="31" t="s">
-        <v>2284</v>
+        <v>2283</v>
       </c>
       <c r="D665" s="27"/>
       <c r="E665" s="27" t="s">
@@ -27907,13 +27902,13 @@
     </row>
     <row r="666" spans="1:11" s="24" customFormat="1" ht="30">
       <c r="A666" s="27" t="s">
-        <v>2285</v>
+        <v>2284</v>
       </c>
       <c r="B666" s="28" t="s">
         <v>706</v>
       </c>
       <c r="C666" s="31" t="s">
-        <v>2286</v>
+        <v>2285</v>
       </c>
       <c r="D666" s="35"/>
       <c r="E666" s="35" t="s">
@@ -27967,7 +27962,7 @@
         <v>706</v>
       </c>
       <c r="C668" s="31" t="s">
-        <v>2287</v>
+        <v>2286</v>
       </c>
       <c r="D668" s="27"/>
       <c r="E668" s="27" t="s">
@@ -28050,7 +28045,7 @@
         <v>706</v>
       </c>
       <c r="C671" s="31" t="s">
-        <v>2288</v>
+        <v>2287</v>
       </c>
       <c r="D671" s="27"/>
       <c r="E671" s="27" t="s">
@@ -28066,7 +28061,7 @@
         <v>17</v>
       </c>
       <c r="I671" s="29" t="s">
-        <v>2319</v>
+        <v>2318</v>
       </c>
       <c r="J671" s="27"/>
       <c r="K671" s="27"/>
@@ -28262,13 +28257,13 @@
     </row>
     <row r="679" spans="1:11" s="24" customFormat="1" ht="30">
       <c r="A679" s="27" t="s">
-        <v>2289</v>
+        <v>2288</v>
       </c>
       <c r="B679" s="28" t="s">
         <v>706</v>
       </c>
       <c r="C679" s="31" t="s">
-        <v>2290</v>
+        <v>2289</v>
       </c>
       <c r="D679" s="35"/>
       <c r="E679" s="27" t="s">
@@ -28392,7 +28387,7 @@
         <v>17</v>
       </c>
       <c r="I683" s="37" t="s">
-        <v>2322</v>
+        <v>2321</v>
       </c>
       <c r="J683" s="44"/>
       <c r="K683" s="27"/>
@@ -28448,23 +28443,23 @@
         <v>17</v>
       </c>
       <c r="I685" s="29" t="s">
-        <v>2291</v>
+        <v>2290</v>
       </c>
       <c r="J685" s="27"/>
       <c r="K685" s="27"/>
     </row>
     <row r="686" spans="1:11" s="24" customFormat="1" ht="45">
       <c r="A686" s="28" t="s">
-        <v>2292</v>
+        <v>2291</v>
       </c>
       <c r="B686" s="28" t="s">
         <v>706</v>
       </c>
       <c r="C686" s="37" t="s">
+        <v>2292</v>
+      </c>
+      <c r="D686" s="37" t="s">
         <v>2293</v>
-      </c>
-      <c r="D686" s="37" t="s">
-        <v>2294</v>
       </c>
       <c r="E686" s="27" t="s">
         <v>19</v>
@@ -28517,7 +28512,7 @@
         <v>706</v>
       </c>
       <c r="C688" s="31" t="s">
-        <v>2295</v>
+        <v>2294</v>
       </c>
       <c r="D688" s="27"/>
       <c r="E688" s="27" t="s">
@@ -28544,7 +28539,7 @@
         <v>706</v>
       </c>
       <c r="C689" s="31" t="s">
-        <v>2296</v>
+        <v>2295</v>
       </c>
       <c r="D689" s="27"/>
       <c r="E689" s="27" t="s">
@@ -28571,7 +28566,7 @@
         <v>706</v>
       </c>
       <c r="C690" s="31" t="s">
-        <v>2297</v>
+        <v>2296</v>
       </c>
       <c r="D690" s="27"/>
       <c r="E690" s="27" t="s">
@@ -28722,7 +28717,7 @@
         <v>17</v>
       </c>
       <c r="I695" s="29" t="s">
-        <v>2325</v>
+        <v>2324</v>
       </c>
       <c r="J695" s="27"/>
       <c r="K695" s="27"/>
@@ -28843,7 +28838,7 @@
         <v>802</v>
       </c>
       <c r="C700" s="31" t="s">
-        <v>2191</v>
+        <v>2190</v>
       </c>
       <c r="D700" s="27"/>
       <c r="E700" s="27" t="s">
@@ -28870,7 +28865,7 @@
         <v>802</v>
       </c>
       <c r="C701" s="31" t="s">
-        <v>2192</v>
+        <v>2191</v>
       </c>
       <c r="D701" s="27"/>
       <c r="E701" s="27" t="s">
@@ -28897,7 +28892,7 @@
         <v>802</v>
       </c>
       <c r="C702" s="31" t="s">
-        <v>2193</v>
+        <v>2192</v>
       </c>
       <c r="D702" s="27"/>
       <c r="E702" s="27" t="s">
@@ -28924,7 +28919,7 @@
         <v>802</v>
       </c>
       <c r="C703" s="31" t="s">
-        <v>2194</v>
+        <v>2193</v>
       </c>
       <c r="D703" s="27"/>
       <c r="E703" s="27" t="s">
@@ -28951,7 +28946,7 @@
         <v>802</v>
       </c>
       <c r="C704" s="31" t="s">
-        <v>2195</v>
+        <v>2194</v>
       </c>
       <c r="D704" s="27"/>
       <c r="E704" s="27" t="s">
@@ -28978,7 +28973,7 @@
         <v>802</v>
       </c>
       <c r="C705" s="31" t="s">
-        <v>2196</v>
+        <v>2195</v>
       </c>
       <c r="D705" s="27"/>
       <c r="E705" s="27" t="s">
@@ -29410,7 +29405,7 @@
         <v>802</v>
       </c>
       <c r="C721" s="31" t="s">
-        <v>2197</v>
+        <v>2196</v>
       </c>
       <c r="D721" s="27"/>
       <c r="E721" s="27" t="s">
@@ -29437,7 +29432,7 @@
         <v>802</v>
       </c>
       <c r="C722" s="31" t="s">
-        <v>2198</v>
+        <v>2197</v>
       </c>
       <c r="D722" s="27"/>
       <c r="E722" s="27" t="s">
@@ -29464,7 +29459,7 @@
         <v>802</v>
       </c>
       <c r="C723" s="31" t="s">
-        <v>2199</v>
+        <v>2198</v>
       </c>
       <c r="D723" s="27"/>
       <c r="E723" s="27" t="s">
@@ -29491,7 +29486,7 @@
         <v>802</v>
       </c>
       <c r="C724" s="31" t="s">
-        <v>2200</v>
+        <v>2199</v>
       </c>
       <c r="D724" s="27"/>
       <c r="E724" s="27" t="s">
@@ -29518,7 +29513,7 @@
         <v>802</v>
       </c>
       <c r="C725" s="31" t="s">
-        <v>2201</v>
+        <v>2200</v>
       </c>
       <c r="D725" s="27"/>
       <c r="E725" s="27" t="s">
@@ -29545,7 +29540,7 @@
         <v>802</v>
       </c>
       <c r="C726" s="31" t="s">
-        <v>2202</v>
+        <v>2201</v>
       </c>
       <c r="D726" s="27"/>
       <c r="E726" s="27" t="s">
@@ -29572,7 +29567,7 @@
         <v>802</v>
       </c>
       <c r="C727" s="31" t="s">
-        <v>2203</v>
+        <v>2202</v>
       </c>
       <c r="D727" s="27"/>
       <c r="E727" s="27" t="s">
@@ -29626,7 +29621,7 @@
         <v>802</v>
       </c>
       <c r="C729" s="31" t="s">
-        <v>2204</v>
+        <v>2203</v>
       </c>
       <c r="D729" s="27"/>
       <c r="E729" s="27" t="s">
@@ -29653,7 +29648,7 @@
         <v>802</v>
       </c>
       <c r="C730" s="31" t="s">
-        <v>2205</v>
+        <v>2204</v>
       </c>
       <c r="D730" s="27"/>
       <c r="E730" s="27" t="s">
@@ -29680,7 +29675,7 @@
         <v>802</v>
       </c>
       <c r="C731" s="31" t="s">
-        <v>2206</v>
+        <v>2205</v>
       </c>
       <c r="D731" s="27"/>
       <c r="E731" s="27" t="s">
@@ -30085,7 +30080,7 @@
         <v>802</v>
       </c>
       <c r="C746" s="31" t="s">
-        <v>2207</v>
+        <v>2206</v>
       </c>
       <c r="D746" s="27"/>
       <c r="E746" s="27" t="s">
@@ -30220,7 +30215,7 @@
         <v>802</v>
       </c>
       <c r="C751" s="31" t="s">
-        <v>2208</v>
+        <v>2207</v>
       </c>
       <c r="D751" s="27"/>
       <c r="E751" s="27" t="s">
@@ -30247,7 +30242,7 @@
         <v>802</v>
       </c>
       <c r="C752" s="31" t="s">
-        <v>2209</v>
+        <v>2208</v>
       </c>
       <c r="D752" s="27"/>
       <c r="E752" s="27" t="s">
@@ -30328,7 +30323,7 @@
         <v>802</v>
       </c>
       <c r="C755" s="31" t="s">
-        <v>2210</v>
+        <v>2209</v>
       </c>
       <c r="D755" s="27"/>
       <c r="E755" s="27" t="s">
@@ -30382,7 +30377,7 @@
         <v>802</v>
       </c>
       <c r="C757" s="31" t="s">
-        <v>2211</v>
+        <v>2210</v>
       </c>
       <c r="D757" s="27"/>
       <c r="E757" s="27" t="s">
@@ -30436,7 +30431,7 @@
         <v>802</v>
       </c>
       <c r="C759" s="31" t="s">
-        <v>2212</v>
+        <v>2211</v>
       </c>
       <c r="D759" s="27"/>
       <c r="E759" s="27" t="s">
@@ -30490,7 +30485,7 @@
         <v>802</v>
       </c>
       <c r="C761" s="31" t="s">
-        <v>2213</v>
+        <v>2212</v>
       </c>
       <c r="D761" s="27"/>
       <c r="E761" s="27" t="s">
@@ -30517,7 +30512,7 @@
         <v>802</v>
       </c>
       <c r="C762" s="31" t="s">
-        <v>2214</v>
+        <v>2213</v>
       </c>
       <c r="D762" s="27"/>
       <c r="E762" s="27" t="s">
@@ -30544,7 +30539,7 @@
         <v>802</v>
       </c>
       <c r="C763" s="31" t="s">
-        <v>2215</v>
+        <v>2214</v>
       </c>
       <c r="D763" s="27"/>
       <c r="E763" s="27" t="s">
@@ -30571,7 +30566,7 @@
         <v>802</v>
       </c>
       <c r="C764" s="31" t="s">
-        <v>2216</v>
+        <v>2215</v>
       </c>
       <c r="D764" s="27"/>
       <c r="E764" s="27" t="s">
@@ -30598,7 +30593,7 @@
         <v>802</v>
       </c>
       <c r="C765" s="31" t="s">
-        <v>2217</v>
+        <v>2216</v>
       </c>
       <c r="D765" s="27"/>
       <c r="E765" s="27" t="s">
@@ -30625,7 +30620,7 @@
         <v>802</v>
       </c>
       <c r="C766" s="31" t="s">
-        <v>2218</v>
+        <v>2217</v>
       </c>
       <c r="D766" s="27"/>
       <c r="E766" s="27" t="s">
@@ -30652,7 +30647,7 @@
         <v>802</v>
       </c>
       <c r="C767" s="31" t="s">
-        <v>2219</v>
+        <v>2218</v>
       </c>
       <c r="D767" s="27"/>
       <c r="E767" s="27" t="s">
@@ -30679,7 +30674,7 @@
         <v>802</v>
       </c>
       <c r="C768" s="31" t="s">
-        <v>2220</v>
+        <v>2219</v>
       </c>
       <c r="D768" s="27"/>
       <c r="E768" s="27" t="s">
@@ -30706,7 +30701,7 @@
         <v>802</v>
       </c>
       <c r="C769" s="31" t="s">
-        <v>2221</v>
+        <v>2220</v>
       </c>
       <c r="D769" s="27"/>
       <c r="E769" s="27" t="s">
@@ -30733,7 +30728,7 @@
         <v>802</v>
       </c>
       <c r="C770" s="31" t="s">
-        <v>2222</v>
+        <v>2221</v>
       </c>
       <c r="D770" s="27"/>
       <c r="E770" s="27" t="s">
@@ -30760,7 +30755,7 @@
         <v>802</v>
       </c>
       <c r="C771" s="31" t="s">
-        <v>2223</v>
+        <v>2222</v>
       </c>
       <c r="D771" s="27"/>
       <c r="E771" s="27" t="s">
@@ -30787,7 +30782,7 @@
         <v>802</v>
       </c>
       <c r="C772" s="31" t="s">
-        <v>2224</v>
+        <v>2223</v>
       </c>
       <c r="D772" s="27"/>
       <c r="E772" s="27" t="s">
@@ -30976,7 +30971,7 @@
         <v>802</v>
       </c>
       <c r="C779" s="31" t="s">
-        <v>2225</v>
+        <v>2224</v>
       </c>
       <c r="D779" s="27"/>
       <c r="E779" s="27" t="s">
@@ -31003,7 +30998,7 @@
         <v>802</v>
       </c>
       <c r="C780" s="31" t="s">
-        <v>2226</v>
+        <v>2225</v>
       </c>
       <c r="D780" s="27"/>
       <c r="E780" s="27" t="s">
@@ -31030,7 +31025,7 @@
         <v>802</v>
       </c>
       <c r="C781" s="31" t="s">
-        <v>2227</v>
+        <v>2226</v>
       </c>
       <c r="D781" s="27"/>
       <c r="E781" s="27" t="s">
@@ -31057,7 +31052,7 @@
         <v>802</v>
       </c>
       <c r="C782" s="31" t="s">
-        <v>2228</v>
+        <v>2227</v>
       </c>
       <c r="D782" s="27"/>
       <c r="E782" s="27" t="s">
@@ -31084,7 +31079,7 @@
         <v>802</v>
       </c>
       <c r="C783" s="31" t="s">
-        <v>2229</v>
+        <v>2228</v>
       </c>
       <c r="D783" s="27"/>
       <c r="E783" s="27" t="s">
@@ -31111,7 +31106,7 @@
         <v>802</v>
       </c>
       <c r="C784" s="31" t="s">
-        <v>2230</v>
+        <v>2229</v>
       </c>
       <c r="D784" s="27"/>
       <c r="E784" s="27" t="s">
@@ -31165,7 +31160,7 @@
         <v>802</v>
       </c>
       <c r="C786" s="31" t="s">
-        <v>2231</v>
+        <v>2230</v>
       </c>
       <c r="D786" s="27"/>
       <c r="E786" s="27" t="s">
@@ -31192,7 +31187,7 @@
         <v>802</v>
       </c>
       <c r="C787" s="31" t="s">
-        <v>2232</v>
+        <v>2231</v>
       </c>
       <c r="D787" s="27"/>
       <c r="E787" s="27" t="s">
@@ -31219,7 +31214,7 @@
         <v>802</v>
       </c>
       <c r="C788" s="31" t="s">
-        <v>2233</v>
+        <v>2232</v>
       </c>
       <c r="D788" s="27"/>
       <c r="E788" s="27" t="s">
@@ -31246,7 +31241,7 @@
         <v>802</v>
       </c>
       <c r="C789" s="31" t="s">
-        <v>2234</v>
+        <v>2233</v>
       </c>
       <c r="D789" s="27"/>
       <c r="E789" s="27" t="s">
@@ -31273,7 +31268,7 @@
         <v>802</v>
       </c>
       <c r="C790" s="31" t="s">
-        <v>2235</v>
+        <v>2234</v>
       </c>
       <c r="D790" s="27"/>
       <c r="E790" s="27" t="s">
@@ -31300,7 +31295,7 @@
         <v>802</v>
       </c>
       <c r="C791" s="31" t="s">
-        <v>2236</v>
+        <v>2235</v>
       </c>
       <c r="D791" s="27"/>
       <c r="E791" s="27" t="s">
@@ -31327,7 +31322,7 @@
         <v>802</v>
       </c>
       <c r="C792" s="31" t="s">
-        <v>2237</v>
+        <v>2236</v>
       </c>
       <c r="D792" s="27"/>
       <c r="E792" s="27" t="s">
@@ -31354,7 +31349,7 @@
         <v>802</v>
       </c>
       <c r="C793" s="31" t="s">
-        <v>2238</v>
+        <v>2237</v>
       </c>
       <c r="D793" s="27"/>
       <c r="E793" s="27" t="s">
@@ -31381,7 +31376,7 @@
         <v>802</v>
       </c>
       <c r="C794" s="31" t="s">
-        <v>2239</v>
+        <v>2238</v>
       </c>
       <c r="D794" s="27"/>
       <c r="E794" s="27" t="s">
@@ -31408,7 +31403,7 @@
         <v>802</v>
       </c>
       <c r="C795" s="31" t="s">
-        <v>2240</v>
+        <v>2239</v>
       </c>
       <c r="D795" s="27"/>
       <c r="E795" s="27" t="s">
@@ -31435,7 +31430,7 @@
         <v>802</v>
       </c>
       <c r="C796" s="31" t="s">
-        <v>2241</v>
+        <v>2240</v>
       </c>
       <c r="D796" s="27"/>
       <c r="E796" s="27" t="s">
@@ -31462,7 +31457,7 @@
         <v>802</v>
       </c>
       <c r="C797" s="31" t="s">
-        <v>2242</v>
+        <v>2241</v>
       </c>
       <c r="D797" s="27"/>
       <c r="E797" s="27" t="s">
@@ -31489,7 +31484,7 @@
         <v>802</v>
       </c>
       <c r="C798" s="31" t="s">
-        <v>2243</v>
+        <v>2242</v>
       </c>
       <c r="D798" s="27"/>
       <c r="E798" s="27" t="s">
@@ -31516,7 +31511,7 @@
         <v>802</v>
       </c>
       <c r="C799" s="31" t="s">
-        <v>2244</v>
+        <v>2243</v>
       </c>
       <c r="D799" s="27"/>
       <c r="E799" s="27" t="s">
@@ -31543,7 +31538,7 @@
         <v>802</v>
       </c>
       <c r="C800" s="31" t="s">
-        <v>2245</v>
+        <v>2244</v>
       </c>
       <c r="D800" s="27"/>
       <c r="E800" s="27" t="s">
@@ -31570,7 +31565,7 @@
         <v>802</v>
       </c>
       <c r="C801" s="31" t="s">
-        <v>2246</v>
+        <v>2245</v>
       </c>
       <c r="D801" s="27"/>
       <c r="E801" s="27" t="s">
@@ -31597,7 +31592,7 @@
         <v>802</v>
       </c>
       <c r="C802" s="31" t="s">
-        <v>2247</v>
+        <v>2246</v>
       </c>
       <c r="D802" s="27"/>
       <c r="E802" s="27" t="s">
@@ -31624,7 +31619,7 @@
         <v>802</v>
       </c>
       <c r="C803" s="31" t="s">
-        <v>2248</v>
+        <v>2247</v>
       </c>
       <c r="D803" s="27"/>
       <c r="E803" s="27" t="s">
@@ -31651,7 +31646,7 @@
         <v>802</v>
       </c>
       <c r="C804" s="31" t="s">
-        <v>2249</v>
+        <v>2248</v>
       </c>
       <c r="D804" s="27"/>
       <c r="E804" s="27" t="s">
@@ -31678,7 +31673,7 @@
         <v>802</v>
       </c>
       <c r="C805" s="31" t="s">
-        <v>2250</v>
+        <v>2249</v>
       </c>
       <c r="D805" s="27"/>
       <c r="E805" s="27" t="s">
@@ -31705,7 +31700,7 @@
         <v>802</v>
       </c>
       <c r="C806" s="31" t="s">
-        <v>2251</v>
+        <v>2250</v>
       </c>
       <c r="D806" s="27"/>
       <c r="E806" s="27" t="s">
@@ -31732,7 +31727,7 @@
         <v>802</v>
       </c>
       <c r="C807" s="31" t="s">
-        <v>2252</v>
+        <v>2251</v>
       </c>
       <c r="D807" s="27"/>
       <c r="E807" s="27" t="s">
@@ -31759,7 +31754,7 @@
         <v>802</v>
       </c>
       <c r="C808" s="31" t="s">
-        <v>2253</v>
+        <v>2252</v>
       </c>
       <c r="D808" s="27"/>
       <c r="E808" s="27" t="s">
@@ -31786,7 +31781,7 @@
         <v>802</v>
       </c>
       <c r="C809" s="31" t="s">
-        <v>2254</v>
+        <v>2253</v>
       </c>
       <c r="D809" s="27"/>
       <c r="E809" s="27" t="s">
@@ -32407,7 +32402,7 @@
         <v>802</v>
       </c>
       <c r="C832" s="31" t="s">
-        <v>2476</v>
+        <v>2474</v>
       </c>
       <c r="D832" s="27"/>
       <c r="E832" s="27" t="s">
@@ -33406,7 +33401,7 @@
         <v>802</v>
       </c>
       <c r="C869" s="31" t="s">
-        <v>2298</v>
+        <v>2297</v>
       </c>
       <c r="D869" s="27"/>
       <c r="E869" s="27" t="s">
@@ -33514,7 +33509,7 @@
         <v>802</v>
       </c>
       <c r="C873" s="31" t="s">
-        <v>2477</v>
+        <v>2475</v>
       </c>
       <c r="D873" s="27"/>
       <c r="E873" s="27" t="s">
@@ -33595,7 +33590,7 @@
         <v>802</v>
       </c>
       <c r="C876" s="31" t="s">
-        <v>2478</v>
+        <v>2476</v>
       </c>
       <c r="D876" s="27"/>
       <c r="E876" s="27" t="s">
@@ -35647,7 +35642,7 @@
         <v>1054</v>
       </c>
       <c r="C952" s="42" t="s">
-        <v>2479</v>
+        <v>2477</v>
       </c>
       <c r="D952" s="35"/>
       <c r="E952" s="27" t="s">
@@ -35674,7 +35669,7 @@
         <v>1054</v>
       </c>
       <c r="C953" s="31" t="s">
-        <v>2255</v>
+        <v>2254</v>
       </c>
       <c r="D953" s="27"/>
       <c r="E953" s="27" t="s">
@@ -35701,7 +35696,7 @@
         <v>1054</v>
       </c>
       <c r="C954" s="31" t="s">
-        <v>2256</v>
+        <v>2255</v>
       </c>
       <c r="D954" s="27"/>
       <c r="E954" s="27" t="s">
@@ -35755,7 +35750,7 @@
         <v>1054</v>
       </c>
       <c r="C956" s="31" t="s">
-        <v>2257</v>
+        <v>2256</v>
       </c>
       <c r="D956" s="27"/>
       <c r="E956" s="27" t="s">
@@ -35782,7 +35777,7 @@
         <v>1054</v>
       </c>
       <c r="C957" s="31" t="s">
-        <v>2258</v>
+        <v>2257</v>
       </c>
       <c r="D957" s="27"/>
       <c r="E957" s="27" t="s">
@@ -35809,7 +35804,7 @@
         <v>1054</v>
       </c>
       <c r="C958" s="31" t="s">
-        <v>2259</v>
+        <v>2258</v>
       </c>
       <c r="D958" s="27"/>
       <c r="E958" s="27" t="s">
@@ -35836,7 +35831,7 @@
         <v>1054</v>
       </c>
       <c r="C959" s="31" t="s">
-        <v>2260</v>
+        <v>2259</v>
       </c>
       <c r="D959" s="27"/>
       <c r="E959" s="27" t="s">
@@ -35863,7 +35858,7 @@
         <v>1054</v>
       </c>
       <c r="C960" s="31" t="s">
-        <v>2261</v>
+        <v>2260</v>
       </c>
       <c r="D960" s="27"/>
       <c r="E960" s="27" t="s">
@@ -36241,7 +36236,7 @@
         <v>1075</v>
       </c>
       <c r="C974" s="31" t="s">
-        <v>2262</v>
+        <v>2261</v>
       </c>
       <c r="D974" s="27"/>
       <c r="E974" s="27" t="s">
@@ -36608,7 +36603,7 @@
         <v>17</v>
       </c>
       <c r="I987" s="29" t="s">
-        <v>2318</v>
+        <v>2317</v>
       </c>
       <c r="J987" s="27"/>
       <c r="K987" s="27"/>
@@ -37053,7 +37048,7 @@
         <v>1106</v>
       </c>
       <c r="C1004" s="31" t="s">
-        <v>2480</v>
+        <v>2478</v>
       </c>
       <c r="D1004" s="27"/>
       <c r="E1004" s="27" t="s">
@@ -37069,7 +37064,7 @@
         <v>17</v>
       </c>
       <c r="I1004" s="29" t="s">
-        <v>2485</v>
+        <v>2483</v>
       </c>
       <c r="J1004" s="27"/>
       <c r="K1004" s="27"/>
@@ -37892,7 +37887,7 @@
         <v>1106</v>
       </c>
       <c r="C1035" s="31" t="s">
-        <v>2486</v>
+        <v>2484</v>
       </c>
       <c r="D1035" s="27"/>
       <c r="E1035" s="27" t="s">
@@ -37935,7 +37930,7 @@
         <v>17</v>
       </c>
       <c r="I1036" s="29" t="s">
-        <v>2324</v>
+        <v>2323</v>
       </c>
       <c r="J1036" s="27"/>
       <c r="K1036" s="27"/>
@@ -38245,7 +38240,7 @@
         <v>1106</v>
       </c>
       <c r="C1048" s="31" t="s">
-        <v>2487</v>
+        <v>2485</v>
       </c>
       <c r="D1048" s="27"/>
       <c r="E1048" s="27" t="s">
@@ -38261,7 +38256,7 @@
         <v>17</v>
       </c>
       <c r="I1048" s="29" t="s">
-        <v>2299</v>
+        <v>2298</v>
       </c>
       <c r="J1048" s="27"/>
       <c r="K1048" s="27"/>
@@ -38274,7 +38269,7 @@
         <v>1106</v>
       </c>
       <c r="C1049" s="31" t="s">
-        <v>2300</v>
+        <v>2299</v>
       </c>
       <c r="D1049" s="27"/>
       <c r="E1049" s="27" t="s">
@@ -38301,7 +38296,7 @@
         <v>1106</v>
       </c>
       <c r="C1050" s="31" t="s">
-        <v>2488</v>
+        <v>2486</v>
       </c>
       <c r="D1050" s="27"/>
       <c r="E1050" s="27" t="s">
@@ -39273,7 +39268,7 @@
         <v>7</v>
       </c>
       <c r="C1086" s="31" t="s">
-        <v>2327</v>
+        <v>2326</v>
       </c>
       <c r="D1086" s="27"/>
       <c r="E1086" s="27" t="s">
@@ -39300,7 +39295,7 @@
         <v>7</v>
       </c>
       <c r="C1087" s="31" t="s">
-        <v>2328</v>
+        <v>2327</v>
       </c>
       <c r="D1087" s="27"/>
       <c r="E1087" s="27" t="s">
@@ -39321,16 +39316,16 @@
     </row>
     <row r="1088" spans="1:11" s="24" customFormat="1" ht="30">
       <c r="A1088" s="51" t="s">
-        <v>2396</v>
+        <v>2395</v>
       </c>
       <c r="B1088" s="47">
         <v>7</v>
       </c>
       <c r="C1088" s="42" t="s">
-        <v>2403</v>
+        <v>2402</v>
       </c>
       <c r="D1088" s="51" t="s">
-        <v>2389</v>
+        <v>2388</v>
       </c>
       <c r="E1088" s="27" t="s">
         <v>22</v>
@@ -39350,16 +39345,16 @@
     </row>
     <row r="1089" spans="1:11" s="24" customFormat="1" ht="30">
       <c r="A1089" s="51" t="s">
-        <v>2397</v>
+        <v>2396</v>
       </c>
       <c r="B1089" s="47">
         <v>7</v>
       </c>
       <c r="C1089" s="42" t="s">
-        <v>2404</v>
+        <v>2403</v>
       </c>
       <c r="D1089" s="51" t="s">
-        <v>2390</v>
+        <v>2389</v>
       </c>
       <c r="E1089" s="27" t="s">
         <v>22</v>
@@ -39379,16 +39374,16 @@
     </row>
     <row r="1090" spans="1:11" s="24" customFormat="1" ht="30">
       <c r="A1090" s="51" t="s">
-        <v>2398</v>
+        <v>2397</v>
       </c>
       <c r="B1090" s="47">
         <v>7</v>
       </c>
       <c r="C1090" s="42" t="s">
-        <v>2405</v>
+        <v>2404</v>
       </c>
       <c r="D1090" s="51" t="s">
-        <v>2391</v>
+        <v>2390</v>
       </c>
       <c r="E1090" s="27" t="s">
         <v>22</v>
@@ -39408,16 +39403,16 @@
     </row>
     <row r="1091" spans="1:11" s="24" customFormat="1" ht="30">
       <c r="A1091" s="51" t="s">
-        <v>2399</v>
+        <v>2398</v>
       </c>
       <c r="B1091" s="47">
         <v>7</v>
       </c>
       <c r="C1091" s="42" t="s">
-        <v>2406</v>
+        <v>2405</v>
       </c>
       <c r="D1091" s="51" t="s">
-        <v>2392</v>
+        <v>2391</v>
       </c>
       <c r="E1091" s="27" t="s">
         <v>22</v>
@@ -39437,16 +39432,16 @@
     </row>
     <row r="1092" spans="1:11" s="24" customFormat="1" ht="30">
       <c r="A1092" s="51" t="s">
-        <v>2400</v>
+        <v>2399</v>
       </c>
       <c r="B1092" s="47">
         <v>7</v>
       </c>
       <c r="C1092" s="42" t="s">
-        <v>2407</v>
+        <v>2406</v>
       </c>
       <c r="D1092" s="51" t="s">
-        <v>2393</v>
+        <v>2392</v>
       </c>
       <c r="E1092" s="27" t="s">
         <v>22</v>
@@ -39466,16 +39461,16 @@
     </row>
     <row r="1093" spans="1:11" s="24" customFormat="1" ht="30">
       <c r="A1093" s="51" t="s">
-        <v>2401</v>
+        <v>2400</v>
       </c>
       <c r="B1093" s="47">
         <v>7</v>
       </c>
       <c r="C1093" s="42" t="s">
-        <v>2408</v>
+        <v>2407</v>
       </c>
       <c r="D1093" s="51" t="s">
-        <v>2394</v>
+        <v>2393</v>
       </c>
       <c r="E1093" s="27" t="s">
         <v>22</v>
@@ -39495,16 +39490,16 @@
     </row>
     <row r="1094" spans="1:11" s="24" customFormat="1" ht="30">
       <c r="A1094" s="51" t="s">
-        <v>2402</v>
+        <v>2401</v>
       </c>
       <c r="B1094" s="47">
         <v>7</v>
       </c>
       <c r="C1094" s="42" t="s">
-        <v>2409</v>
+        <v>2408</v>
       </c>
       <c r="D1094" s="51" t="s">
-        <v>2395</v>
+        <v>2394</v>
       </c>
       <c r="E1094" s="27" t="s">
         <v>22</v>
@@ -39524,16 +39519,16 @@
     </row>
     <row r="1095" spans="1:11" s="24" customFormat="1" ht="30">
       <c r="A1095" s="51" t="s">
-        <v>2431</v>
+        <v>2430</v>
       </c>
       <c r="B1095" s="47">
         <v>7</v>
       </c>
       <c r="C1095" s="42" t="s">
-        <v>2438</v>
+        <v>2437</v>
       </c>
       <c r="D1095" s="51" t="s">
-        <v>2424</v>
+        <v>2423</v>
       </c>
       <c r="E1095" s="27" t="s">
         <v>22</v>
@@ -39553,16 +39548,16 @@
     </row>
     <row r="1096" spans="1:11" s="24" customFormat="1" ht="30">
       <c r="A1096" s="51" t="s">
-        <v>2432</v>
+        <v>2431</v>
       </c>
       <c r="B1096" s="47">
         <v>7</v>
       </c>
       <c r="C1096" s="42" t="s">
-        <v>2439</v>
+        <v>2438</v>
       </c>
       <c r="D1096" s="51" t="s">
-        <v>2425</v>
+        <v>2424</v>
       </c>
       <c r="E1096" s="27" t="s">
         <v>22</v>
@@ -39582,16 +39577,16 @@
     </row>
     <row r="1097" spans="1:11" s="24" customFormat="1" ht="30">
       <c r="A1097" s="51" t="s">
-        <v>2433</v>
+        <v>2432</v>
       </c>
       <c r="B1097" s="47">
         <v>7</v>
       </c>
       <c r="C1097" s="42" t="s">
-        <v>2440</v>
+        <v>2439</v>
       </c>
       <c r="D1097" s="51" t="s">
-        <v>2426</v>
+        <v>2425</v>
       </c>
       <c r="E1097" s="27" t="s">
         <v>22</v>
@@ -39611,16 +39606,16 @@
     </row>
     <row r="1098" spans="1:11" s="24" customFormat="1" ht="30">
       <c r="A1098" s="51" t="s">
-        <v>2434</v>
+        <v>2433</v>
       </c>
       <c r="B1098" s="47">
         <v>7</v>
       </c>
       <c r="C1098" s="42" t="s">
-        <v>2441</v>
+        <v>2440</v>
       </c>
       <c r="D1098" s="51" t="s">
-        <v>2427</v>
+        <v>2426</v>
       </c>
       <c r="E1098" s="27" t="s">
         <v>22</v>
@@ -39640,16 +39635,16 @@
     </row>
     <row r="1099" spans="1:11" s="24" customFormat="1" ht="30">
       <c r="A1099" s="51" t="s">
-        <v>2435</v>
+        <v>2434</v>
       </c>
       <c r="B1099" s="47">
         <v>7</v>
       </c>
       <c r="C1099" s="42" t="s">
-        <v>2442</v>
+        <v>2441</v>
       </c>
       <c r="D1099" s="51" t="s">
-        <v>2428</v>
+        <v>2427</v>
       </c>
       <c r="E1099" s="27" t="s">
         <v>22</v>
@@ -39669,16 +39664,16 @@
     </row>
     <row r="1100" spans="1:11" s="24" customFormat="1" ht="30">
       <c r="A1100" s="51" t="s">
-        <v>2436</v>
+        <v>2435</v>
       </c>
       <c r="B1100" s="47">
         <v>7</v>
       </c>
       <c r="C1100" s="42" t="s">
-        <v>2443</v>
+        <v>2442</v>
       </c>
       <c r="D1100" s="51" t="s">
-        <v>2429</v>
+        <v>2428</v>
       </c>
       <c r="E1100" s="27" t="s">
         <v>22</v>
@@ -39698,16 +39693,16 @@
     </row>
     <row r="1101" spans="1:11" s="24" customFormat="1" ht="30">
       <c r="A1101" s="51" t="s">
-        <v>2437</v>
+        <v>2436</v>
       </c>
       <c r="B1101" s="47">
         <v>7</v>
       </c>
       <c r="C1101" s="42" t="s">
-        <v>2444</v>
+        <v>2443</v>
       </c>
       <c r="D1101" s="51" t="s">
-        <v>2430</v>
+        <v>2429</v>
       </c>
       <c r="E1101" s="27" t="s">
         <v>22</v>
@@ -39727,16 +39722,16 @@
     </row>
     <row r="1102" spans="1:11" s="24" customFormat="1" ht="45">
       <c r="A1102" s="51" t="s">
-        <v>2450</v>
+        <v>2449</v>
       </c>
       <c r="B1102" s="47">
         <v>7</v>
       </c>
       <c r="C1102" s="42" t="s">
-        <v>2451</v>
+        <v>2450</v>
       </c>
       <c r="D1102" s="51" t="s">
-        <v>2449</v>
+        <v>2448</v>
       </c>
       <c r="E1102" s="27" t="s">
         <v>22</v>
@@ -39751,7 +39746,7 @@
         <v>20</v>
       </c>
       <c r="I1102" s="48" t="s">
-        <v>2317</v>
+        <v>2316</v>
       </c>
       <c r="J1102" s="27"/>
       <c r="K1102" s="27"/>
@@ -39782,23 +39777,23 @@
         <v>20</v>
       </c>
       <c r="I1103" s="29" t="s">
-        <v>2317</v>
+        <v>2316</v>
       </c>
       <c r="J1103" s="44"/>
       <c r="K1103" s="27"/>
     </row>
     <row r="1104" spans="1:11" s="24" customFormat="1" ht="45">
       <c r="A1104" s="27" t="s">
-        <v>2301</v>
+        <v>2300</v>
       </c>
       <c r="B1104" s="38">
         <v>7</v>
       </c>
       <c r="C1104" s="37" t="s">
+        <v>2301</v>
+      </c>
+      <c r="D1104" s="27" t="s">
         <v>2302</v>
-      </c>
-      <c r="D1104" s="27" t="s">
-        <v>2303</v>
       </c>
       <c r="E1104" s="27" t="s">
         <v>22</v>
@@ -39813,7 +39808,7 @@
         <v>20</v>
       </c>
       <c r="I1104" s="29" t="s">
-        <v>2317</v>
+        <v>2316</v>
       </c>
       <c r="J1104" s="27"/>
       <c r="K1104" s="27"/>
@@ -39855,7 +39850,7 @@
         <v>7</v>
       </c>
       <c r="C1106" s="37" t="s">
-        <v>2304</v>
+        <v>2303</v>
       </c>
       <c r="D1106" s="27" t="s">
         <v>2133</v>
@@ -39873,7 +39868,7 @@
         <v>20</v>
       </c>
       <c r="I1106" s="29" t="s">
-        <v>2317</v>
+        <v>2316</v>
       </c>
       <c r="J1106" s="44"/>
       <c r="K1106" s="27"/>
@@ -39904,7 +39899,7 @@
         <v>21</v>
       </c>
       <c r="I1107" s="29" t="s">
-        <v>2317</v>
+        <v>2316</v>
       </c>
       <c r="J1107" s="27"/>
       <c r="K1107" s="27"/>
@@ -39935,7 +39930,7 @@
         <v>20</v>
       </c>
       <c r="I1108" s="29" t="s">
-        <v>2317</v>
+        <v>2316</v>
       </c>
       <c r="J1108" s="27"/>
       <c r="K1108" s="27"/>
@@ -39966,7 +39961,7 @@
         <v>20</v>
       </c>
       <c r="I1109" s="29" t="s">
-        <v>2317</v>
+        <v>2316</v>
       </c>
       <c r="J1109" s="27"/>
       <c r="K1109" s="27"/>
@@ -39997,7 +39992,7 @@
         <v>20</v>
       </c>
       <c r="I1110" s="29" t="s">
-        <v>2317</v>
+        <v>2316</v>
       </c>
       <c r="J1110" s="27"/>
       <c r="K1110" s="27"/>
@@ -40010,7 +40005,7 @@
         <v>7</v>
       </c>
       <c r="C1111" s="31" t="s">
-        <v>2305</v>
+        <v>2304</v>
       </c>
       <c r="D1111" s="27" t="s">
         <v>1210</v>
@@ -40028,7 +40023,7 @@
         <v>20</v>
       </c>
       <c r="I1111" s="29" t="s">
-        <v>2317</v>
+        <v>2316</v>
       </c>
       <c r="J1111" s="27"/>
       <c r="K1111" s="27"/>
@@ -40044,7 +40039,7 @@
         <v>2135</v>
       </c>
       <c r="D1112" s="27" t="s">
-        <v>2306</v>
+        <v>2305</v>
       </c>
       <c r="E1112" s="27" t="s">
         <v>22</v>
@@ -40070,10 +40065,10 @@
         <v>7</v>
       </c>
       <c r="C1113" s="42" t="s">
-        <v>2307</v>
+        <v>2306</v>
       </c>
       <c r="D1113" s="27" t="s">
-        <v>2306</v>
+        <v>2305</v>
       </c>
       <c r="E1113" s="27" t="s">
         <v>22</v>
@@ -40088,14 +40083,14 @@
         <v>20</v>
       </c>
       <c r="I1113" s="29" t="s">
-        <v>2317</v>
+        <v>2316</v>
       </c>
       <c r="J1113" s="45"/>
       <c r="K1113" s="27"/>
     </row>
     <row r="1114" spans="1:11" s="24" customFormat="1" ht="45">
       <c r="A1114" s="27" t="s">
-        <v>2308</v>
+        <v>2307</v>
       </c>
       <c r="B1114" s="43">
         <v>7</v>
@@ -40104,7 +40099,7 @@
         <v>2137</v>
       </c>
       <c r="D1114" s="27" t="s">
-        <v>2309</v>
+        <v>2308</v>
       </c>
       <c r="E1114" s="27" t="s">
         <v>22</v>
@@ -40119,23 +40114,23 @@
         <v>20</v>
       </c>
       <c r="I1114" s="29" t="s">
-        <v>2317</v>
+        <v>2316</v>
       </c>
       <c r="J1114" s="45"/>
       <c r="K1114" s="27"/>
     </row>
     <row r="1115" spans="1:11" s="24" customFormat="1" ht="45">
       <c r="A1115" s="27" t="s">
-        <v>2310</v>
+        <v>2309</v>
       </c>
       <c r="B1115" s="43">
         <v>7</v>
       </c>
       <c r="C1115" s="42" t="s">
-        <v>2326</v>
+        <v>2325</v>
       </c>
       <c r="D1115" s="27" t="s">
-        <v>2309</v>
+        <v>2308</v>
       </c>
       <c r="E1115" s="27" t="s">
         <v>22</v>
@@ -40150,23 +40145,23 @@
         <v>20</v>
       </c>
       <c r="I1115" s="29" t="s">
-        <v>2317</v>
+        <v>2316</v>
       </c>
       <c r="J1115" s="45"/>
       <c r="K1115" s="27"/>
     </row>
     <row r="1116" spans="1:11" s="24" customFormat="1" ht="45">
       <c r="A1116" s="27" t="s">
-        <v>2311</v>
+        <v>2310</v>
       </c>
       <c r="B1116" s="43">
         <v>7</v>
       </c>
       <c r="C1116" s="42" t="s">
-        <v>2312</v>
+        <v>2311</v>
       </c>
       <c r="D1116" s="27" t="s">
-        <v>2309</v>
+        <v>2308</v>
       </c>
       <c r="E1116" s="27" t="s">
         <v>22</v>
@@ -40181,23 +40176,23 @@
         <v>20</v>
       </c>
       <c r="I1116" s="29" t="s">
-        <v>2317</v>
+        <v>2316</v>
       </c>
       <c r="J1116" s="45"/>
       <c r="K1116" s="27"/>
     </row>
     <row r="1117" spans="1:11" s="24" customFormat="1" ht="45">
       <c r="A1117" s="27" t="s">
-        <v>2313</v>
+        <v>2312</v>
       </c>
       <c r="B1117" s="43">
         <v>7</v>
       </c>
       <c r="C1117" s="42" t="s">
-        <v>2314</v>
+        <v>2313</v>
       </c>
       <c r="D1117" s="27" t="s">
-        <v>2309</v>
+        <v>2308</v>
       </c>
       <c r="E1117" s="27" t="s">
         <v>22</v>
@@ -40212,7 +40207,7 @@
         <v>20</v>
       </c>
       <c r="I1117" s="29" t="s">
-        <v>2317</v>
+        <v>2316</v>
       </c>
       <c r="J1117" s="45"/>
       <c r="K1117" s="27"/>
@@ -40252,7 +40247,7 @@
         <v>7</v>
       </c>
       <c r="C1119" s="31" t="s">
-        <v>2489</v>
+        <v>2487</v>
       </c>
       <c r="D1119" s="27"/>
       <c r="E1119" s="27" t="s">
@@ -40295,7 +40290,7 @@
         <v>20</v>
       </c>
       <c r="I1120" s="29" t="s">
-        <v>2317</v>
+        <v>2316</v>
       </c>
       <c r="J1120" s="27"/>
       <c r="K1120" s="27"/>
@@ -40355,7 +40350,7 @@
         <v>20</v>
       </c>
       <c r="I1122" s="29" t="s">
-        <v>2317</v>
+        <v>2316</v>
       </c>
       <c r="J1122" s="27"/>
       <c r="K1122" s="27"/>
@@ -40467,7 +40462,7 @@
         <v>20</v>
       </c>
       <c r="I1126" s="29" t="s">
-        <v>2317</v>
+        <v>2316</v>
       </c>
       <c r="J1126" s="44"/>
       <c r="K1126" s="27"/>
@@ -40588,7 +40583,7 @@
         <v>7</v>
       </c>
       <c r="C1131" s="31" t="s">
-        <v>2490</v>
+        <v>2488</v>
       </c>
       <c r="D1131" s="27" t="s">
         <v>2149</v>
@@ -40606,7 +40601,7 @@
         <v>20</v>
       </c>
       <c r="I1131" s="29" t="s">
-        <v>2317</v>
+        <v>2316</v>
       </c>
       <c r="J1131" s="44"/>
       <c r="K1131" s="27"/>
@@ -40619,7 +40614,7 @@
         <v>7</v>
       </c>
       <c r="C1132" s="31" t="s">
-        <v>2491</v>
+        <v>2489</v>
       </c>
       <c r="D1132" s="27"/>
       <c r="E1132" s="27" t="s">
@@ -41207,16 +41202,16 @@
     </row>
     <row r="1154" spans="1:11" s="24" customFormat="1" ht="45">
       <c r="A1154" s="51" t="s">
-        <v>2469</v>
+        <v>2468</v>
       </c>
       <c r="B1154" s="47">
         <v>7</v>
       </c>
       <c r="C1154" s="42" t="s">
-        <v>2472</v>
+        <v>2471</v>
       </c>
       <c r="D1154" s="51" t="s">
-        <v>2471</v>
+        <v>2470</v>
       </c>
       <c r="E1154" s="27" t="s">
         <v>22</v>
@@ -41234,18 +41229,18 @@
       <c r="J1154" s="27"/>
       <c r="K1154" s="27"/>
     </row>
-    <row r="1155" spans="1:11" s="24" customFormat="1" ht="45">
+    <row r="1155" spans="1:11" s="24" customFormat="1" ht="30">
       <c r="A1155" s="51" t="s">
-        <v>2470</v>
+        <v>2469</v>
       </c>
       <c r="B1155" s="47">
         <v>7</v>
       </c>
       <c r="C1155" s="42" t="s">
-        <v>2473</v>
+        <v>2472</v>
       </c>
       <c r="D1155" s="51" t="s">
-        <v>2471</v>
+        <v>2470</v>
       </c>
       <c r="E1155" s="27" t="s">
         <v>22</v>
@@ -41257,11 +41252,9 @@
         <v>15</v>
       </c>
       <c r="H1155" s="52" t="s">
-        <v>20</v>
-      </c>
-      <c r="I1155" s="48" t="s">
-        <v>2317</v>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="I1155" s="48"/>
       <c r="J1155" s="27"/>
       <c r="K1155" s="27"/>
     </row>
@@ -41678,7 +41671,7 @@
         <v>7</v>
       </c>
       <c r="C1171" s="31" t="s">
-        <v>2492</v>
+        <v>2490</v>
       </c>
       <c r="D1171" s="27"/>
       <c r="E1171" s="27" t="s">
@@ -41699,13 +41692,13 @@
     </row>
     <row r="1172" spans="1:11" s="24" customFormat="1" ht="45">
       <c r="A1172" s="51" t="s">
-        <v>2481</v>
+        <v>2479</v>
       </c>
       <c r="B1172" s="47">
         <v>7</v>
       </c>
       <c r="C1172" s="42" t="s">
-        <v>2483</v>
+        <v>2481</v>
       </c>
       <c r="D1172" s="46"/>
       <c r="E1172" s="27" t="s">
@@ -41721,20 +41714,20 @@
         <v>20</v>
       </c>
       <c r="I1172" s="48" t="s">
-        <v>2317</v>
+        <v>2316</v>
       </c>
       <c r="J1172" s="27"/>
       <c r="K1172" s="27"/>
     </row>
     <row r="1173" spans="1:11" s="24" customFormat="1" ht="45">
       <c r="A1173" s="51" t="s">
-        <v>2482</v>
+        <v>2480</v>
       </c>
       <c r="B1173" s="47">
         <v>7</v>
       </c>
       <c r="C1173" s="42" t="s">
-        <v>2484</v>
+        <v>2482</v>
       </c>
       <c r="D1173" s="46"/>
       <c r="E1173" s="27" t="s">
@@ -41750,7 +41743,7 @@
         <v>20</v>
       </c>
       <c r="I1173" s="48" t="s">
-        <v>2317</v>
+        <v>2316</v>
       </c>
       <c r="J1173" s="27"/>
       <c r="K1173" s="27"/>
@@ -41763,7 +41756,7 @@
         <v>7</v>
       </c>
       <c r="C1174" s="31" t="s">
-        <v>2493</v>
+        <v>2491</v>
       </c>
       <c r="D1174" s="27"/>
       <c r="E1174" s="27" t="s">
@@ -42390,12 +42383,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -42404,7 +42391,7 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F2EA47BB262D974097182E2CA8AB13E1" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="74597e8d9e42e7e4fc8eda6d37675aa2">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4aeb20c0e3442673af7ee10786458764">
     <xsd:element name="properties">
@@ -42453,21 +42440,13 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{923F65C5-DEAB-400B-AA1F-124F40EE10AC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6D33261-F3C6-4621-88F1-D76E5ABE1865}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
@@ -42475,7 +42454,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EDB2DE12-5EF6-4CF2-820D-5F9FE329E08E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -42488,4 +42467,18 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/internal/2005/internalDocumentation"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{923F65C5-DEAB-400B-AA1F-124F40EE10AC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
[MS-OUTSPS]: Fix watchman warnings
</commit_message>
<xml_diff>
--- a/SharePoint/Docs/MS-OUTSPS/MS-OUTSPS_RequirementSpecification.xlsx
+++ b/SharePoint/Docs/MS-OUTSPS/MS-OUTSPS_RequirementSpecification.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="16925"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8116" uniqueCount="2494">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8117" uniqueCount="2495">
   <si>
     <t>Req ID</t>
   </si>
@@ -7975,9 +7975,6 @@
     <t>[In Common Schema][vti_versionhistory:]The vti_versionhistory field can be absent from the schema.</t>
   </si>
   <si>
-    <t xml:space="preserve">[In Appointment-Specific Schema]If the fAllDayEvent property is 1, the Duration MUST be 86340 seconds (1 minute less than 24 hours) when the appointment iss not a single appointment. </t>
-  </si>
-  <si>
     <t>MS-OUTSPS_R8631</t>
   </si>
   <si>
@@ -8092,6 +8089,12 @@
   </si>
   <si>
     <t>[In Common Schema]Unless stated otherwise[Attachments, Categories, Created, Modified, ReplicationID, vti_versionhistory], all fields in this section[ContentTypeId, ID, owshiddenversion] MUST be present on all item types&lt;20&gt; and contain valid data.</t>
+  </si>
+  <si>
+    <t>MS-OUTSPS_R698:i</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[In Appointment-Specific Schema]If the fAllDayEvent property is 1, the Duration MUST be 86340 seconds (1 minute less than 24 hours) when the appointment is not a single appointment. </t>
   </si>
 </sst>
 </file>
@@ -8432,21 +8435,6 @@
     <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -8470,6 +8458,21 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -10171,120 +10174,120 @@
       </c>
     </row>
     <row r="4" spans="1:9" ht="21">
-      <c r="A4" s="53" t="s">
+      <c r="A4" s="61" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="53"/>
-      <c r="C4" s="53"/>
-      <c r="D4" s="53"/>
-      <c r="E4" s="53"/>
-      <c r="F4" s="53"/>
-      <c r="G4" s="53"/>
+      <c r="B4" s="61"/>
+      <c r="C4" s="61"/>
+      <c r="D4" s="61"/>
+      <c r="E4" s="61"/>
+      <c r="F4" s="61"/>
+      <c r="G4" s="61"/>
     </row>
     <row r="5" spans="1:9">
       <c r="A5" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="54" t="s">
+      <c r="B5" s="62" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="55"/>
-      <c r="D5" s="55"/>
-      <c r="E5" s="55"/>
-      <c r="F5" s="55"/>
-      <c r="G5" s="55"/>
-      <c r="H5" s="55"/>
-      <c r="I5" s="55"/>
+      <c r="C5" s="63"/>
+      <c r="D5" s="63"/>
+      <c r="E5" s="63"/>
+      <c r="F5" s="63"/>
+      <c r="G5" s="63"/>
+      <c r="H5" s="63"/>
+      <c r="I5" s="63"/>
     </row>
     <row r="6" spans="1:9">
       <c r="A6" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="56" t="s">
+      <c r="B6" s="64" t="s">
         <v>30</v>
       </c>
-      <c r="C6" s="56"/>
-      <c r="D6" s="56"/>
-      <c r="E6" s="56"/>
-      <c r="F6" s="56"/>
-      <c r="G6" s="56"/>
-      <c r="H6" s="56"/>
-      <c r="I6" s="56"/>
+      <c r="C6" s="64"/>
+      <c r="D6" s="64"/>
+      <c r="E6" s="64"/>
+      <c r="F6" s="64"/>
+      <c r="G6" s="64"/>
+      <c r="H6" s="64"/>
+      <c r="I6" s="64"/>
     </row>
     <row r="7" spans="1:9">
       <c r="A7" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="B7" s="57" t="s">
+      <c r="B7" s="65" t="s">
         <v>1273</v>
       </c>
-      <c r="C7" s="57"/>
-      <c r="D7" s="57"/>
-      <c r="E7" s="57"/>
-      <c r="F7" s="57"/>
-      <c r="G7" s="57"/>
-      <c r="H7" s="57"/>
-      <c r="I7" s="57"/>
+      <c r="C7" s="65"/>
+      <c r="D7" s="65"/>
+      <c r="E7" s="65"/>
+      <c r="F7" s="65"/>
+      <c r="G7" s="65"/>
+      <c r="H7" s="65"/>
+      <c r="I7" s="65"/>
     </row>
     <row r="8" spans="1:9">
       <c r="A8" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="57" t="s">
+      <c r="B8" s="65" t="s">
         <v>1274</v>
       </c>
-      <c r="C8" s="57"/>
-      <c r="D8" s="57"/>
-      <c r="E8" s="57"/>
-      <c r="F8" s="57"/>
-      <c r="G8" s="57"/>
-      <c r="H8" s="57"/>
-      <c r="I8" s="57"/>
+      <c r="C8" s="65"/>
+      <c r="D8" s="65"/>
+      <c r="E8" s="65"/>
+      <c r="F8" s="65"/>
+      <c r="G8" s="65"/>
+      <c r="H8" s="65"/>
+      <c r="I8" s="65"/>
     </row>
     <row r="9" spans="1:9" ht="78.75" customHeight="1">
       <c r="A9" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="61" t="s">
+      <c r="B9" s="56" t="s">
         <v>33</v>
       </c>
-      <c r="C9" s="62"/>
-      <c r="D9" s="62"/>
-      <c r="E9" s="62"/>
-      <c r="F9" s="62"/>
-      <c r="G9" s="62"/>
-      <c r="H9" s="62"/>
-      <c r="I9" s="62"/>
+      <c r="C9" s="57"/>
+      <c r="D9" s="57"/>
+      <c r="E9" s="57"/>
+      <c r="F9" s="57"/>
+      <c r="G9" s="57"/>
+      <c r="H9" s="57"/>
+      <c r="I9" s="57"/>
     </row>
     <row r="10" spans="1:9" ht="33.75" customHeight="1">
       <c r="A10" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="61" t="s">
+      <c r="B10" s="56" t="s">
         <v>1275</v>
       </c>
-      <c r="C10" s="62"/>
-      <c r="D10" s="62"/>
-      <c r="E10" s="62"/>
-      <c r="F10" s="62"/>
-      <c r="G10" s="62"/>
-      <c r="H10" s="62"/>
-      <c r="I10" s="62"/>
+      <c r="C10" s="57"/>
+      <c r="D10" s="57"/>
+      <c r="E10" s="57"/>
+      <c r="F10" s="57"/>
+      <c r="G10" s="57"/>
+      <c r="H10" s="57"/>
+      <c r="I10" s="57"/>
     </row>
     <row r="11" spans="1:9">
       <c r="A11" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="58" t="s">
+      <c r="B11" s="53" t="s">
         <v>36</v>
       </c>
-      <c r="C11" s="58"/>
-      <c r="D11" s="58"/>
-      <c r="E11" s="58"/>
-      <c r="F11" s="58"/>
-      <c r="G11" s="58"/>
-      <c r="H11" s="58"/>
-      <c r="I11" s="58"/>
+      <c r="C11" s="53"/>
+      <c r="D11" s="53"/>
+      <c r="E11" s="53"/>
+      <c r="F11" s="53"/>
+      <c r="G11" s="53"/>
+      <c r="H11" s="53"/>
+      <c r="I11" s="53"/>
     </row>
     <row r="12" spans="1:9">
       <c r="A12" s="21" t="s">
@@ -10296,12 +10299,12 @@
       <c r="C12" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="D12" s="63"/>
-      <c r="E12" s="63"/>
-      <c r="F12" s="63"/>
-      <c r="G12" s="63"/>
-      <c r="H12" s="63"/>
-      <c r="I12" s="63"/>
+      <c r="D12" s="58"/>
+      <c r="E12" s="58"/>
+      <c r="F12" s="58"/>
+      <c r="G12" s="58"/>
+      <c r="H12" s="58"/>
+      <c r="I12" s="58"/>
     </row>
     <row r="13" spans="1:9" ht="15" customHeight="1">
       <c r="A13" s="22" t="s">
@@ -10313,12 +10316,12 @@
       <c r="C13" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="D13" s="64"/>
-      <c r="E13" s="64"/>
-      <c r="F13" s="64"/>
-      <c r="G13" s="64"/>
-      <c r="H13" s="64"/>
-      <c r="I13" s="64"/>
+      <c r="D13" s="59"/>
+      <c r="E13" s="59"/>
+      <c r="F13" s="59"/>
+      <c r="G13" s="59"/>
+      <c r="H13" s="59"/>
+      <c r="I13" s="59"/>
     </row>
     <row r="14" spans="1:9">
       <c r="A14" s="22" t="s">
@@ -10330,12 +10333,12 @@
       <c r="C14" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="D14" s="64"/>
-      <c r="E14" s="64"/>
-      <c r="F14" s="64"/>
-      <c r="G14" s="64"/>
-      <c r="H14" s="64"/>
-      <c r="I14" s="64"/>
+      <c r="D14" s="59"/>
+      <c r="E14" s="59"/>
+      <c r="F14" s="59"/>
+      <c r="G14" s="59"/>
+      <c r="H14" s="59"/>
+      <c r="I14" s="59"/>
     </row>
     <row r="15" spans="1:9">
       <c r="A15" s="23" t="s">
@@ -10347,57 +10350,57 @@
       <c r="C15" s="16" t="s">
         <v>1276</v>
       </c>
-      <c r="D15" s="65"/>
-      <c r="E15" s="65"/>
-      <c r="F15" s="65"/>
-      <c r="G15" s="65"/>
-      <c r="H15" s="65"/>
-      <c r="I15" s="65"/>
+      <c r="D15" s="60"/>
+      <c r="E15" s="60"/>
+      <c r="F15" s="60"/>
+      <c r="G15" s="60"/>
+      <c r="H15" s="60"/>
+      <c r="I15" s="60"/>
     </row>
     <row r="16" spans="1:9" ht="30" customHeight="1">
       <c r="A16" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="B16" s="58" t="s">
+      <c r="B16" s="53" t="s">
         <v>37</v>
       </c>
-      <c r="C16" s="58"/>
-      <c r="D16" s="58"/>
-      <c r="E16" s="58"/>
-      <c r="F16" s="58"/>
-      <c r="G16" s="58"/>
-      <c r="H16" s="58"/>
-      <c r="I16" s="58"/>
+      <c r="C16" s="53"/>
+      <c r="D16" s="53"/>
+      <c r="E16" s="53"/>
+      <c r="F16" s="53"/>
+      <c r="G16" s="53"/>
+      <c r="H16" s="53"/>
+      <c r="I16" s="53"/>
     </row>
     <row r="17" spans="1:11" ht="64.5" customHeight="1">
       <c r="A17" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="B17" s="59" t="s">
+      <c r="B17" s="54" t="s">
         <v>1277</v>
       </c>
-      <c r="C17" s="60"/>
-      <c r="D17" s="60"/>
-      <c r="E17" s="60"/>
-      <c r="F17" s="60"/>
-      <c r="G17" s="60"/>
-      <c r="H17" s="60"/>
-      <c r="I17" s="60"/>
+      <c r="C17" s="55"/>
+      <c r="D17" s="55"/>
+      <c r="E17" s="55"/>
+      <c r="F17" s="55"/>
+      <c r="G17" s="55"/>
+      <c r="H17" s="55"/>
+      <c r="I17" s="55"/>
     </row>
     <row r="18" spans="1:11" ht="30" customHeight="1">
       <c r="A18" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="B18" s="58" t="s">
+      <c r="B18" s="53" t="s">
         <v>32</v>
       </c>
-      <c r="C18" s="58"/>
-      <c r="D18" s="58"/>
-      <c r="E18" s="58"/>
-      <c r="F18" s="58"/>
-      <c r="G18" s="58"/>
-      <c r="H18" s="58"/>
-      <c r="I18" s="58"/>
+      <c r="C18" s="53"/>
+      <c r="D18" s="53"/>
+      <c r="E18" s="53"/>
+      <c r="F18" s="53"/>
+      <c r="G18" s="53"/>
+      <c r="H18" s="53"/>
+      <c r="I18" s="53"/>
     </row>
     <row r="19" spans="1:11" ht="30">
       <c r="A19" s="3" t="s">
@@ -22747,7 +22750,7 @@
         <v>578</v>
       </c>
       <c r="C475" s="31" t="s">
-        <v>2492</v>
+        <v>2491</v>
       </c>
       <c r="D475" s="27"/>
       <c r="E475" s="27" t="s">
@@ -24421,7 +24424,7 @@
         <v>644</v>
       </c>
       <c r="C537" s="31" t="s">
-        <v>2493</v>
+        <v>2492</v>
       </c>
       <c r="D537" s="27"/>
       <c r="E537" s="27" t="s">
@@ -26909,7 +26912,7 @@
         <v>706</v>
       </c>
       <c r="C629" s="31" t="s">
-        <v>2463</v>
+        <v>2494</v>
       </c>
       <c r="D629" s="27"/>
       <c r="E629" s="27" t="s">
@@ -26930,13 +26933,13 @@
     </row>
     <row r="630" spans="1:11" s="24" customFormat="1" ht="30">
       <c r="A630" s="51" t="s">
-        <v>2464</v>
+        <v>2463</v>
       </c>
       <c r="B630" s="47" t="s">
         <v>706</v>
       </c>
       <c r="C630" s="31" t="s">
-        <v>2465</v>
+        <v>2464</v>
       </c>
       <c r="D630" s="46"/>
       <c r="E630" s="27" t="s">
@@ -26963,7 +26966,7 @@
         <v>706</v>
       </c>
       <c r="C631" s="31" t="s">
-        <v>2466</v>
+        <v>2465</v>
       </c>
       <c r="D631" s="27"/>
       <c r="E631" s="27" t="s">
@@ -27422,7 +27425,7 @@
         <v>706</v>
       </c>
       <c r="C648" s="31" t="s">
-        <v>2467</v>
+        <v>2466</v>
       </c>
       <c r="D648" s="27"/>
       <c r="E648" s="27" t="s">
@@ -27557,7 +27560,7 @@
         <v>706</v>
       </c>
       <c r="C653" s="31" t="s">
-        <v>2473</v>
+        <v>2472</v>
       </c>
       <c r="D653" s="27"/>
       <c r="E653" s="27" t="s">
@@ -32402,7 +32405,7 @@
         <v>802</v>
       </c>
       <c r="C832" s="31" t="s">
-        <v>2474</v>
+        <v>2473</v>
       </c>
       <c r="D832" s="27"/>
       <c r="E832" s="27" t="s">
@@ -33509,7 +33512,7 @@
         <v>802</v>
       </c>
       <c r="C873" s="31" t="s">
-        <v>2475</v>
+        <v>2474</v>
       </c>
       <c r="D873" s="27"/>
       <c r="E873" s="27" t="s">
@@ -33590,7 +33593,7 @@
         <v>802</v>
       </c>
       <c r="C876" s="31" t="s">
-        <v>2476</v>
+        <v>2475</v>
       </c>
       <c r="D876" s="27"/>
       <c r="E876" s="27" t="s">
@@ -35642,7 +35645,7 @@
         <v>1054</v>
       </c>
       <c r="C952" s="42" t="s">
-        <v>2477</v>
+        <v>2476</v>
       </c>
       <c r="D952" s="35"/>
       <c r="E952" s="27" t="s">
@@ -37048,7 +37051,7 @@
         <v>1106</v>
       </c>
       <c r="C1004" s="31" t="s">
-        <v>2478</v>
+        <v>2477</v>
       </c>
       <c r="D1004" s="27"/>
       <c r="E1004" s="27" t="s">
@@ -37064,7 +37067,7 @@
         <v>17</v>
       </c>
       <c r="I1004" s="29" t="s">
-        <v>2483</v>
+        <v>2482</v>
       </c>
       <c r="J1004" s="27"/>
       <c r="K1004" s="27"/>
@@ -37887,7 +37890,7 @@
         <v>1106</v>
       </c>
       <c r="C1035" s="31" t="s">
-        <v>2484</v>
+        <v>2483</v>
       </c>
       <c r="D1035" s="27"/>
       <c r="E1035" s="27" t="s">
@@ -38240,7 +38243,7 @@
         <v>1106</v>
       </c>
       <c r="C1048" s="31" t="s">
-        <v>2485</v>
+        <v>2484</v>
       </c>
       <c r="D1048" s="27"/>
       <c r="E1048" s="27" t="s">
@@ -38296,7 +38299,7 @@
         <v>1106</v>
       </c>
       <c r="C1050" s="31" t="s">
-        <v>2486</v>
+        <v>2485</v>
       </c>
       <c r="D1050" s="27"/>
       <c r="E1050" s="27" t="s">
@@ -40082,9 +40085,7 @@
       <c r="H1113" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="I1113" s="29" t="s">
-        <v>2316</v>
-      </c>
+      <c r="I1113" s="29"/>
       <c r="J1113" s="45"/>
       <c r="K1113" s="27"/>
     </row>
@@ -40247,7 +40248,7 @@
         <v>7</v>
       </c>
       <c r="C1119" s="31" t="s">
-        <v>2487</v>
+        <v>2486</v>
       </c>
       <c r="D1119" s="27"/>
       <c r="E1119" s="27" t="s">
@@ -40583,7 +40584,7 @@
         <v>7</v>
       </c>
       <c r="C1131" s="31" t="s">
-        <v>2488</v>
+        <v>2487</v>
       </c>
       <c r="D1131" s="27" t="s">
         <v>2149</v>
@@ -40614,7 +40615,7 @@
         <v>7</v>
       </c>
       <c r="C1132" s="31" t="s">
-        <v>2489</v>
+        <v>2488</v>
       </c>
       <c r="D1132" s="27"/>
       <c r="E1132" s="27" t="s">
@@ -41202,16 +41203,16 @@
     </row>
     <row r="1154" spans="1:11" s="24" customFormat="1" ht="45">
       <c r="A1154" s="51" t="s">
-        <v>2468</v>
+        <v>2467</v>
       </c>
       <c r="B1154" s="47">
         <v>7</v>
       </c>
       <c r="C1154" s="42" t="s">
-        <v>2471</v>
+        <v>2470</v>
       </c>
       <c r="D1154" s="51" t="s">
-        <v>2470</v>
+        <v>2469</v>
       </c>
       <c r="E1154" s="27" t="s">
         <v>22</v>
@@ -41231,16 +41232,16 @@
     </row>
     <row r="1155" spans="1:11" s="24" customFormat="1" ht="30">
       <c r="A1155" s="51" t="s">
-        <v>2469</v>
+        <v>2468</v>
       </c>
       <c r="B1155" s="47">
         <v>7</v>
       </c>
       <c r="C1155" s="42" t="s">
-        <v>2472</v>
+        <v>2471</v>
       </c>
       <c r="D1155" s="51" t="s">
-        <v>2470</v>
+        <v>2469</v>
       </c>
       <c r="E1155" s="27" t="s">
         <v>22</v>
@@ -41671,7 +41672,7 @@
         <v>7</v>
       </c>
       <c r="C1171" s="31" t="s">
-        <v>2490</v>
+        <v>2489</v>
       </c>
       <c r="D1171" s="27"/>
       <c r="E1171" s="27" t="s">
@@ -41692,15 +41693,17 @@
     </row>
     <row r="1172" spans="1:11" s="24" customFormat="1" ht="45">
       <c r="A1172" s="51" t="s">
-        <v>2479</v>
+        <v>2478</v>
       </c>
       <c r="B1172" s="47">
         <v>7</v>
       </c>
       <c r="C1172" s="42" t="s">
-        <v>2481</v>
-      </c>
-      <c r="D1172" s="46"/>
+        <v>2480</v>
+      </c>
+      <c r="D1172" s="51" t="s">
+        <v>2493</v>
+      </c>
       <c r="E1172" s="27" t="s">
         <v>22</v>
       </c>
@@ -41721,15 +41724,17 @@
     </row>
     <row r="1173" spans="1:11" s="24" customFormat="1" ht="45">
       <c r="A1173" s="51" t="s">
-        <v>2480</v>
+        <v>2479</v>
       </c>
       <c r="B1173" s="47">
         <v>7</v>
       </c>
       <c r="C1173" s="42" t="s">
-        <v>2482</v>
-      </c>
-      <c r="D1173" s="46"/>
+        <v>2481</v>
+      </c>
+      <c r="D1173" s="51" t="s">
+        <v>2493</v>
+      </c>
       <c r="E1173" s="27" t="s">
         <v>22</v>
       </c>
@@ -41756,7 +41761,7 @@
         <v>7</v>
       </c>
       <c r="C1174" s="31" t="s">
-        <v>2491</v>
+        <v>2490</v>
       </c>
       <c r="D1174" s="27"/>
       <c r="E1174" s="27" t="s">
@@ -41785,6 +41790,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A4:G4"/>
+    <mergeCell ref="B5:I5"/>
+    <mergeCell ref="B6:I6"/>
+    <mergeCell ref="B7:I7"/>
+    <mergeCell ref="B8:I8"/>
     <mergeCell ref="B16:I16"/>
     <mergeCell ref="B17:I17"/>
     <mergeCell ref="B18:I18"/>
@@ -41792,11 +41802,6 @@
     <mergeCell ref="B10:I10"/>
     <mergeCell ref="B11:I11"/>
     <mergeCell ref="D12:I15"/>
-    <mergeCell ref="A4:G4"/>
-    <mergeCell ref="B5:I5"/>
-    <mergeCell ref="B6:I6"/>
-    <mergeCell ref="B7:I7"/>
-    <mergeCell ref="B8:I8"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="F687 F1105:F1111 F690:F1103 F24:F684 F1118:F1174">
@@ -41807,7 +41812,7 @@
       <formula>(VLOOKUP(F24,$A$13:$C$16,2,FALSE)="In")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A922:C922 E690:K694 A687 E695:H695 J695:K695 A690:D921 E1048:H1048 J1048:K1048 E696:K1047 J1103:K1103 A1103:C1103 C687:K687 A668:A684 B679:B689 E1118:K1119 E1123:K1125 E1122:H1122 J1122:K1122 E1127:K1130 E1126:H1126 J1126:K1126 E1131:H1131 J1131:K1131 A1105:D1109 E1106:H1109 J1106:K1111 E1105:K1105 E1121:K1121 E1120:H1120 J1120:K1120 E1103:H1103 C668:K684 A1110:H1111 A1114:D1114 E1114:H1117 A923:D1102 E1049:K1102 A24:K667 A1118:D1174 E1132:K1174">
+  <conditionalFormatting sqref="A922:C922 E690:K694 A687 E695:H695 J695:K695 A690:D921 E1048:H1048 J1048:K1048 E696:K1047 J1103:K1103 A1103:C1103 C687:K687 A668:A684 B679:B689 E1118:K1119 E1123:K1125 E1122:H1122 J1122:K1122 E1127:K1130 E1126:H1126 J1126:K1126 E1131:H1131 J1131:K1131 A1105:D1109 E1106:H1109 J1106:K1111 E1105:K1105 E1121:K1121 E1120:H1120 J1120:K1120 E1103:H1103 C668:K684 A1110:H1111 A1114:D1114 E1114:H1117 A923:D1102 E1049:K1102 A24:K667 E1132:K1174 A1118:D1174">
     <cfRule type="expression" dxfId="163" priority="200">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
@@ -41818,7 +41823,7 @@
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A922:C922 E690:I694 A687 E695:H695 A690:D921 E1048:H1048 E696:I1047 A1103:C1103 C687:I687 A668:A684 B679:B689 E1118:I1119 E1123:I1125 E1122:H1122 E1127:I1130 E1126:H1126 E1131:H1131 A1105:D1109 E1106:H1109 E1105:I1105 E1121:I1121 E1120:H1120 E1103:H1103 C668:I684 A1110:H1111 A1114:D1114 E1114:H1117 A923:D1102 E1049:I1102 A24:I667 A1118:D1174 E1132:I1174">
+  <conditionalFormatting sqref="A922:C922 E690:I694 A687 E695:H695 A690:D921 E1048:H1048 E696:I1047 A1103:C1103 C687:I687 A668:A684 B679:B689 E1118:I1119 E1123:I1125 E1122:H1122 E1127:I1130 E1126:H1126 E1131:H1131 A1105:D1109 E1106:H1109 E1105:I1105 E1121:I1121 E1120:H1120 E1103:H1103 C668:I684 A1110:H1111 A1114:D1114 E1114:H1117 A923:D1102 E1049:I1102 A24:I667 E1132:I1174 A1118:D1174">
     <cfRule type="expression" dxfId="160" priority="197">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
@@ -42383,15 +42388,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F2EA47BB262D974097182E2CA8AB13E1" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="74597e8d9e42e7e4fc8eda6d37675aa2">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4aeb20c0e3442673af7ee10786458764">
     <xsd:element name="properties">
@@ -42440,6 +42436,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
   <documentManagement/>
@@ -42447,14 +42452,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6D33261-F3C6-4621-88F1-D76E5ABE1865}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EDB2DE12-5EF6-4CF2-820D-5F9FE329E08E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -42465,6 +42462,14 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/internal/2005/internalDocumentation"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6D33261-F3C6-4621-88F1-D76E5ABE1865}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>